<commit_message>
Finished first week of Global Markets class.
</commit_message>
<xml_diff>
--- a/ClassesTaken/Coursera/2016/InvManagementRice/01GlobalMarkets/GlobalMarkets.xlsx
+++ b/ClassesTaken/Coursera/2016/InvManagementRice/01GlobalMarkets/GlobalMarkets.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
   <si>
     <t>Annuity</t>
   </si>
@@ -46,6 +46,45 @@
   </si>
   <si>
     <t>FutVal</t>
+  </si>
+  <si>
+    <t>APR</t>
+  </si>
+  <si>
+    <t>PeriodRate</t>
+  </si>
+  <si>
+    <t>PerForRate</t>
+  </si>
+  <si>
+    <t>PerRate</t>
+  </si>
+  <si>
+    <t>ContComp</t>
+  </si>
+  <si>
+    <t>Perpetuity</t>
+  </si>
+  <si>
+    <t>GrowthRate</t>
+  </si>
+  <si>
+    <t>AnnGrowthRate</t>
+  </si>
+  <si>
+    <t>Amt</t>
+  </si>
+  <si>
+    <t>CompPer</t>
+  </si>
+  <si>
+    <t>RatePerPeriod</t>
+  </si>
+  <si>
+    <t>TotMult</t>
+  </si>
+  <si>
+    <t>EffPeriods</t>
   </si>
 </sst>
 </file>
@@ -94,8 +133,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -110,15 +169,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -131,8 +210,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E9" totalsRowShown="0">
+  <autoFilter ref="A1:E9"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Annuity"/>
     <tableColumn id="2" name="Rate"/>
@@ -148,9 +227,49 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A49:G52" totalsRowShown="0">
+  <autoFilter ref="A49:G52"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Amt"/>
+    <tableColumn id="2" name="APR"/>
+    <tableColumn id="3" name="CompPer"/>
+    <tableColumn id="4" name="Periods"/>
+    <tableColumn id="5" name="RatePerPeriod">
+      <calculatedColumnFormula>$B50/$C50</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="TotMult">
+      <calculatedColumnFormula>POWER(1+$E50,$D50)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="FutVal">
+      <calculatedColumnFormula>$A50*$F50</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="H19:L20" totalsRowShown="0">
+  <autoFilter ref="H19:L20"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Loan"/>
+    <tableColumn id="2" name="Rate"/>
+    <tableColumn id="3" name="EffPeriods"/>
+    <tableColumn id="4" name="ADF">
+      <calculatedColumnFormula>(1-1/POWER(1+$I20,$J20))/$I20</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Payments">
+      <calculatedColumnFormula>$H20/(1+$K20)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="G1:K5" totalsRowShown="0">
-  <autoFilter ref="G1:K5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="H1:L6" totalsRowShown="0">
+  <autoFilter ref="H1:L6"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Loan"/>
     <tableColumn id="2" name="Rate" dataDxfId="0">
@@ -158,10 +277,10 @@
     </tableColumn>
     <tableColumn id="3" name="Periods"/>
     <tableColumn id="4" name="ADF">
-      <calculatedColumnFormula>(1-1/POWER(1+$H2,$I2))/$H2</calculatedColumnFormula>
+      <calculatedColumnFormula>(1-1/POWER(1+$I2,$J2))/$I2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Payments">
-      <calculatedColumnFormula>$G2/$J2</calculatedColumnFormula>
+      <calculatedColumnFormula>$H2/$K2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -169,17 +288,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="M1:Q3" totalsRowShown="0">
-  <autoFilter ref="M1:Q3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="N1:R3" totalsRowShown="0">
+  <autoFilter ref="N1:R3"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Annuity"/>
     <tableColumn id="2" name="Rate"/>
     <tableColumn id="3" name="Periods"/>
     <tableColumn id="4" name="ACF">
-      <calculatedColumnFormula>(POWER(1+$N2,$O2)-1)/$N2</calculatedColumnFormula>
+      <calculatedColumnFormula>(POWER(1+$O2,$P2)-1)/$O2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="FutVal">
-      <calculatedColumnFormula>$M2*$P2</calculatedColumnFormula>
+      <calculatedColumnFormula>$N2*$Q2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -187,20 +306,99 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="S1:W2" totalsRowShown="0">
-  <autoFilter ref="S1:W2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="T1:X4" totalsRowShown="0">
+  <autoFilter ref="T1:X4"/>
   <tableColumns count="5">
     <tableColumn id="1" name="FutVal"/>
     <tableColumn id="2" name="Rate"/>
     <tableColumn id="3" name="Periods"/>
     <tableColumn id="4" name="ACF">
-      <calculatedColumnFormula>(POWER(1+$T2,$U2)-1)/$T2</calculatedColumnFormula>
+      <calculatedColumnFormula>(POWER(1+$U2,$V2)-1)/$U2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Annuity">
-      <calculatedColumnFormula>$S2/$V2</calculatedColumnFormula>
+      <calculatedColumnFormula>$T2/$W2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A12:E29" totalsRowShown="0">
+  <autoFilter ref="A12:E29"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="APR"/>
+    <tableColumn id="2" name="Periods"/>
+    <tableColumn id="3" name="PeriodRate">
+      <calculatedColumnFormula>$A13/$B13</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="PerForRate"/>
+    <tableColumn id="5" name="PerRate">
+      <calculatedColumnFormula>POWER(1+$C13,$D13)-1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="H12:I13" totalsRowShown="0">
+  <autoFilter ref="H12:I13"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="APR"/>
+    <tableColumn id="2" name="ContComp">
+      <calculatedColumnFormula>EXP($H13)-1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A33:D43" totalsRowShown="0">
+  <autoFilter ref="A33:D43"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Perpetuity"/>
+    <tableColumn id="2" name="Rate"/>
+    <tableColumn id="3" name="GrowthRate"/>
+    <tableColumn id="4" name="PresVal">
+      <calculatedColumnFormula>$A34/($B34-$C34)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A45:F47" totalsRowShown="0">
+  <autoFilter ref="A45:F47"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Annuity"/>
+    <tableColumn id="2" name="Rate"/>
+    <tableColumn id="3" name="AnnGrowthRate"/>
+    <tableColumn id="4" name="Periods"/>
+    <tableColumn id="5" name="ADF">
+      <calculatedColumnFormula>(1-POWER((1+$C46)/(1+$B46),$D46))/($B46-$C46)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="PresVal">
+      <calculatedColumnFormula>$A46*$E46</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="H15:J17" totalsRowShown="0">
+  <autoFilter ref="H15:J17"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Rate"/>
+    <tableColumn id="2" name="Periods"/>
+    <tableColumn id="3" name="PeriodRate">
+      <calculatedColumnFormula>POWER(1+$H16,1/$I16)-1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -526,20 +724,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:AA52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" customWidth="1"/>
-    <col min="17" max="17" width="16" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -555,53 +760,53 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>0</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>1</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>2</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>8</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>8</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>1</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>2</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>7</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:27">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -619,60 +824,67 @@
         <f>$A2*$D2</f>
         <v>9985.64784663305</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>37150</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <f>0.04/12</f>
         <v>3.3333333333333335E-3</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>60</v>
       </c>
-      <c r="J2">
-        <f>(1-1/POWER(1+$H2,$I2))/$H2</f>
+      <c r="K2">
+        <f>(1-1/POWER(1+$I2,$J2))/$I2</f>
         <v>54.299068901235152</v>
       </c>
-      <c r="K2">
-        <f>$G2/$J2</f>
+      <c r="L2">
+        <f>$H2/$K2</f>
         <v>684.17379435312819</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>3000</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>0.05</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>4</v>
       </c>
-      <c r="P2">
-        <f>(POWER(1+$N2,$O2)-1)/$N2</f>
+      <c r="Q2">
+        <f>(POWER(1+$O2,$P2)-1)/$O2</f>
         <v>4.3101250000000002</v>
       </c>
-      <c r="Q2">
-        <f>$M2*$P2</f>
+      <c r="R2">
+        <f>$N2*$Q2</f>
         <v>12930.375</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>1000000</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>0.06</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>35</v>
       </c>
-      <c r="V2">
-        <f>(POWER(1+$T2,$U2)-1)/$T2</f>
+      <c r="W2">
+        <f>(POWER(1+$U2,$V2)-1)/$U2</f>
         <v>111.43477987187251</v>
       </c>
-      <c r="W2">
-        <f>$S2/$V2</f>
+      <c r="X2">
+        <f>$T2/$W2</f>
         <v>8973.8589796632441</v>
       </c>
-    </row>
-    <row r="3" spans="1:23">
+      <c r="Z2">
+        <v>408279.35837032669</v>
+      </c>
+      <c r="AA2">
+        <f>1000000-$Z2</f>
+        <v>591720.64162967331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
@@ -690,44 +902,62 @@
         <f>$A3*$D3</f>
         <v>7091.9010083247213</v>
       </c>
-      <c r="G3" s="1">
+      <c r="F3" s="1"/>
+      <c r="H3" s="1">
         <v>450000</v>
       </c>
-      <c r="H3" s="1">
-        <f t="shared" ref="H2:H3" si="0">0.035/12</f>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3" si="0">0.035/12</f>
         <v>2.9166666666666668E-3</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <f>30*12</f>
         <v>360</v>
       </c>
-      <c r="J3" s="1">
-        <f>(1-1/POWER(1+$H3,$I3))/$H3</f>
+      <c r="K3" s="1">
+        <f>(1-1/POWER(1+$I3,$J3))/$I3</f>
         <v>222.69498496455597</v>
       </c>
-      <c r="K3" s="1">
-        <f>$G3/$J3</f>
+      <c r="L3" s="1">
+        <f>$H3/$K3</f>
         <v>2020.7010951397122</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>5000</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>0.06</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>20</v>
       </c>
-      <c r="P3" s="1">
-        <f>(POWER(1+$N3,$O3)-1)/$N3</f>
+      <c r="Q3" s="1">
+        <f>(POWER(1+$O3,$P3)-1)/$O3</f>
         <v>36.785591203547469</v>
       </c>
-      <c r="Q3" s="1">
-        <f>$M3*$P3</f>
+      <c r="R3" s="1">
+        <f>$N3*$Q3</f>
         <v>183927.95601773734</v>
       </c>
-    </row>
-    <row r="4" spans="1:23">
+      <c r="T3" s="1">
+        <v>25000</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="V3" s="1">
+        <v>5</v>
+      </c>
+      <c r="W3" s="1">
+        <f>(POWER(1+$U3,$V3)-1)/$U3</f>
+        <v>5.866600960000004</v>
+      </c>
+      <c r="X3" s="1">
+        <f>$T3/$W3</f>
+        <v>4261.4113641709118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4" s="1">
         <v>500</v>
       </c>
@@ -745,27 +975,45 @@
         <f>$A4*$D4</f>
         <v>16435.50811963249</v>
       </c>
-      <c r="G4" s="1">
+      <c r="F4" s="1"/>
+      <c r="H4" s="1">
         <v>450000</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <f>0.03/12</f>
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <f>20*12</f>
         <v>240</v>
       </c>
-      <c r="J4" s="1">
-        <f>(1-1/POWER(1+$H4,$I4))/$H4</f>
+      <c r="K4" s="1">
+        <f>(1-1/POWER(1+$I4,$J4))/$I4</f>
         <v>180.31091441247096</v>
       </c>
-      <c r="K4" s="1">
-        <f>$G4/$J4</f>
+      <c r="L4" s="1">
+        <f>$H4/$K4</f>
         <v>2495.6891903426358</v>
       </c>
-    </row>
-    <row r="5" spans="1:23">
+      <c r="T4" s="1">
+        <v>591720.64162967331</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="V4" s="1">
+        <v>35</v>
+      </c>
+      <c r="W4" s="1">
+        <f>(POWER(1+$U4,$V4)-1)/$U4</f>
+        <v>215.71075465018151</v>
+      </c>
+      <c r="X4" s="1">
+        <f>$T4/$W4</f>
+        <v>2743.1207247374737</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
       <c r="A5" s="1">
         <v>600</v>
       </c>
@@ -783,27 +1031,28 @@
         <f>$A5*$D5</f>
         <v>13537.719733059439</v>
       </c>
-      <c r="G5" s="1">
+      <c r="F5" s="1"/>
+      <c r="H5" s="1">
         <v>450000</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <f>0.028/12</f>
         <v>2.3333333333333335E-3</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <f>15*12</f>
         <v>180</v>
       </c>
-      <c r="J5" s="1">
-        <f>(1-1/POWER(1+$H5,$I5))/$H5</f>
+      <c r="K5" s="1">
+        <f>(1-1/POWER(1+$I5,$J5))/$I5</f>
         <v>146.84213508754502</v>
       </c>
-      <c r="K5" s="1">
-        <f>$G5/$J5</f>
+      <c r="L5" s="1">
+        <f>$H5/$K5</f>
         <v>3064.5155066133907</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:27">
       <c r="A6" s="1">
         <v>350</v>
       </c>
@@ -821,15 +1070,890 @@
         <f>$A6*$D6</f>
         <v>14903.111223988719</v>
       </c>
+      <c r="F6" s="1"/>
+      <c r="H6" s="1">
+        <v>90000</v>
+      </c>
+      <c r="I6" s="2">
+        <f>0.035/12</f>
+        <v>2.9166666666666668E-3</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1">
+        <f>(1-1/POWER(1+$I6,$J6))/$I6</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="e">
+        <f>$H6/$K6</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B7" s="1">
+        <f>0.06/12</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>40</v>
+      </c>
+      <c r="D7" s="1">
+        <f>(1-1/POWER(1+$B7,$C7))/$B7</f>
+        <v>36.172227864082075</v>
+      </c>
+      <c r="E7" s="1">
+        <f>$A7*$D7</f>
+        <v>36172.227864082073</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="C8" s="1">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1">
+        <f>(1-1/POWER(1+$B8,$C8))/$B8</f>
+        <v>6.4176577011590128</v>
+      </c>
+      <c r="E8" s="1">
+        <f>$A8*$D8</f>
+        <v>32088.288505795063</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="A9" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="C9" s="1">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1">
+        <f>(1-1/POWER(1+$B9,$C9))/$B9</f>
+        <v>10.273654043021743</v>
+      </c>
+      <c r="E9" s="1">
+        <f>$A9*$D9</f>
+        <v>51368.270215108714</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:27">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="A13">
+        <v>0.04</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f>$A13/$B13</f>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <f>POWER(1+$C13,$D13)-1</f>
+        <v>4.0741542919790819E-2</v>
+      </c>
+      <c r="H13">
+        <v>0.06</v>
+      </c>
+      <c r="I13">
+        <f>EXP($H13)-1</f>
+        <v>6.1836546545359639E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="A14" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="B14" s="1">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1">
+        <f>$A14/$B14</f>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <f>POWER(1+$C14,$D14)-1</f>
+        <v>6.6777777777780045E-3</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="A15" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="B15" s="1">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1">
+        <f>$A15/$B15</f>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1">
+        <f>POWER(1+$C15,$D15)-1</f>
+        <v>1.0033370370370776E-2</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="H15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="A16" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="B16" s="1">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
+        <f>$A16/$B16</f>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>18</v>
+      </c>
+      <c r="E16" s="1">
+        <f>POWER(1+$C16,$D16)-1</f>
+        <v>6.173060355153881E-2</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="H16">
+        <v>0.06</v>
+      </c>
+      <c r="I16">
+        <v>12</v>
+      </c>
+      <c r="J16">
+        <f>POWER(1+$H16,1/$I16)-1</f>
+        <v>4.8675505653430484E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1">
+        <f>$A17/$B17</f>
+        <v>0.03</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1">
+        <f>POWER(1+$C17,$D17)-1</f>
+        <v>6.0899999999999954E-2</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="H17" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="I17" s="1">
+        <v>12</v>
+      </c>
+      <c r="J17" s="1">
+        <f>POWER(1+$H17,1/$I17)-1</f>
+        <v>4.0741237836483535E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1">
+        <f>$A18/$B18</f>
+        <v>0.03</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="1">
+        <f>POWER(1+$C18,$D18)-1</f>
+        <v>1.4889156509221957E-2</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <f>$A19/$B19</f>
+        <v>0.03</v>
+      </c>
+      <c r="D19" s="1">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1">
+        <f>POWER(1+$C19,$D19)-1</f>
+        <v>0.12550880999999992</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="H19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" t="s">
+        <v>4</v>
+      </c>
+      <c r="L19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1">
+        <f>$A20/$B20</f>
+        <v>0.03</v>
+      </c>
+      <c r="D20" s="1">
+        <f>15/6</f>
+        <v>2.5</v>
+      </c>
+      <c r="E20" s="1">
+        <f>POWER(1+$C20,$D20)-1</f>
+        <v>7.6695906140633596E-2</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="H20">
+        <v>4000</v>
+      </c>
+      <c r="I20">
+        <v>0.01</v>
+      </c>
+      <c r="J20">
+        <v>23</v>
+      </c>
+      <c r="K20">
+        <f>(1-1/POWER(1+$I20,$J20))/$I20</f>
+        <v>20.455821130204143</v>
+      </c>
+      <c r="L20">
+        <f>$H20/(1+$K20)</f>
+        <v>186.42959296342445</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <f>$A21/$B21</f>
+        <v>0.02</v>
+      </c>
+      <c r="D21" s="1">
+        <v>4</v>
+      </c>
+      <c r="E21" s="1">
+        <f>POWER(1+$C21,$D21)-1</f>
+        <v>8.2432159999999977E-2</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="B22" s="1">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1">
+        <f>$A22/$B22</f>
+        <v>0.02</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1">
+        <f>POWER(1+$C22,$D22)-1</f>
+        <v>4.0399999999999991E-2</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="B23" s="1">
+        <v>12</v>
+      </c>
+      <c r="C23" s="1">
+        <f>$A23/$B23</f>
+        <v>6.6666666666666671E-3</v>
+      </c>
+      <c r="D23" s="1">
+        <v>6</v>
+      </c>
+      <c r="E23" s="1">
+        <f>POWER(1+$C23,$D23)-1</f>
+        <v>4.067262230132207E-2</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <f>$A24/$B24</f>
+        <v>0.03</v>
+      </c>
+      <c r="D24" s="1">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1">
+        <f>POWER(1+$C24,$D24)-1</f>
+        <v>0.34391637934412178</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="B25" s="1">
+        <v>12</v>
+      </c>
+      <c r="C25" s="1">
+        <f>$A25/$B25</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D25" s="1">
+        <v>12</v>
+      </c>
+      <c r="E25" s="1">
+        <f>POWER(1+$C25,$D25)-1</f>
+        <v>6.1677811864497611E-2</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B26" s="1">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
+        <f>$A26/$B26</f>
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4</v>
+      </c>
+      <c r="E26" s="1">
+        <f>POWER(1+$C26,$D26)-1</f>
+        <v>7.1859031289062791E-2</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="1">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1">
+        <f>$A27/$B27</f>
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2</v>
+      </c>
+      <c r="E27" s="1">
+        <f>POWER(1+$C27,$D27)-1</f>
+        <v>6.6056249999999928E-2</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
+        <f>$A28/$B28</f>
+        <v>0.02</v>
+      </c>
+      <c r="D28" s="1">
+        <v>4</v>
+      </c>
+      <c r="E28" s="1">
+        <f>POWER(1+$C28,$D28)-1</f>
+        <v>8.2432159999999977E-2</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="B29" s="1">
+        <v>12</v>
+      </c>
+      <c r="C29" s="1">
+        <f>$A29/$B29</f>
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1">
+        <f>POWER(1+$C29,$D29)-1</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>1000</v>
+      </c>
+      <c r="B34">
+        <v>0.1</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <f>$A34/($B34-$C34)</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>1000</v>
+      </c>
+      <c r="B35">
+        <v>0.1</v>
+      </c>
+      <c r="C35">
+        <v>0.05</v>
+      </c>
+      <c r="D35">
+        <f>$A35/($B35-$C35)</f>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <f>$A36/($B36-$C36)</f>
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B37" s="1">
+        <v>4.0741237836483535E-3</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <f>$A37/($B37-$C37)</f>
+        <v>245451.5505919425</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="D38" s="1">
+        <f>$A38/($B38-$C38)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1">
+        <v>750</v>
+      </c>
+      <c r="B39" s="1">
+        <v>4.8675505653430484E-3</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <f>$A39/($B39-$C39)</f>
+        <v>154081.60427546428</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1">
+        <v>500</v>
+      </c>
+      <c r="B40" s="1">
+        <v>4.8675505653430484E-3</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1.25E-3</v>
+      </c>
+      <c r="D40" s="1">
+        <f>$A40/($B40-$C40)</f>
+        <v>138215.06872360347</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B41" s="1">
+        <f>0.05/12</f>
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1">
+        <f>$A41/($B41-$C41)</f>
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="1">
+        <v>20000</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1">
+        <f>$A42/($B42-$C42)</f>
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="1">
+        <v>100</v>
+      </c>
+      <c r="B43" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D43" s="1">
+        <f>$A43/($B43-$C43)</f>
+        <v>4999.9999999999991</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <v>90000</v>
+      </c>
+      <c r="B46">
+        <v>0.08</v>
+      </c>
+      <c r="C46">
+        <v>0.05</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="E46">
+        <f>(1-POWER((1+$C46)/(1+$B46),$D46))/($B46-$C46)</f>
+        <v>4.3794737959505428</v>
+      </c>
+      <c r="F46">
+        <f>$A46*$E46</f>
+        <v>394152.64163554885</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="1">
+        <v>1250</v>
+      </c>
+      <c r="B47" s="1">
+        <v>4.8675505653430484E-3</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1.25E-3</v>
+      </c>
+      <c r="D47" s="1">
+        <v>36</v>
+      </c>
+      <c r="E47" s="1">
+        <f>(1-POWER((1+$C47)/(1+$B47),$D47))/($B47-$C47)</f>
+        <v>33.658000442053236</v>
+      </c>
+      <c r="F47" s="1">
+        <f>$A47*$E47</f>
+        <v>42072.500552566547</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50">
+        <v>1000</v>
+      </c>
+      <c r="B50">
+        <v>0.08</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>6</v>
+      </c>
+      <c r="E50">
+        <f>$B50/$C50</f>
+        <v>0.04</v>
+      </c>
+      <c r="F50">
+        <f>POWER(1+$E50,$D50)</f>
+        <v>1.2653190184960004</v>
+      </c>
+      <c r="G50">
+        <f>$A50*$F50</f>
+        <v>1265.3190184960004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="C51" s="1">
+        <v>12</v>
+      </c>
+      <c r="D51" s="1">
+        <v>36</v>
+      </c>
+      <c r="E51" s="1">
+        <f>$B51/$C51</f>
+        <v>6.6666666666666671E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f>POWER(1+$E51,$D51)</f>
+        <v>1.2702370516206511</v>
+      </c>
+      <c r="G51" s="1">
+        <f>$A51*$F51</f>
+        <v>1270.2370516206511</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="1">
+        <v>20000</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1">
+        <v>35</v>
+      </c>
+      <c r="E52" s="1">
+        <f>$B52/$C52</f>
+        <v>0.09</v>
+      </c>
+      <c r="F52" s="1">
+        <f>POWER(1+$E52,$D52)</f>
+        <v>20.413967918516335</v>
+      </c>
+      <c r="G52" s="1">
+        <f>$A52*$F52</f>
+        <v>408279.35837032669</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <tableParts count="4">
+  <tableParts count="11">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Global Markets online class.
</commit_message>
<xml_diff>
--- a/ClassesTaken/Coursera/2016/InvManagementRice/01GlobalMarkets/GlobalMarkets.xlsx
+++ b/ClassesTaken/Coursera/2016/InvManagementRice/01GlobalMarkets/GlobalMarkets.xlsx
@@ -1,15 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Users\marshallfarrier\Workspace\solutions\ClassesTaken\Coursera\2016\InvManagementRice\01GlobalMarkets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17340" yWindow="-21580" windowWidth="31040" windowHeight="20140" tabRatio="500"/>
+    <workbookView xWindow="17340" yWindow="-21576" windowWidth="31044" windowHeight="20136" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="wk01" sheetId="1" r:id="rId1"/>
+    <sheet name="wk02" sheetId="2" r:id="rId2"/>
+    <sheet name="wk03" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="78">
   <si>
     <t>Annuity</t>
   </si>
@@ -85,13 +92,188 @@
   </si>
   <si>
     <t>EffPeriods</t>
+  </si>
+  <si>
+    <t>FaceVal</t>
+  </si>
+  <si>
+    <t>Yrs</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>Nperiods</t>
+  </si>
+  <si>
+    <t>RetPeriods</t>
+  </si>
+  <si>
+    <t>RetPerPeriod</t>
+  </si>
+  <si>
+    <t>CoupPerYr</t>
+  </si>
+  <si>
+    <t>CoupPresVal</t>
+  </si>
+  <si>
+    <t>FacePresVal</t>
+  </si>
+  <si>
+    <t>TotPresVal</t>
+  </si>
+  <si>
+    <t>CoupVal</t>
+  </si>
+  <si>
+    <t>TBillFaceVal</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>Maturity</t>
+  </si>
+  <si>
+    <t>DaysToMat</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>ImpliedPrice</t>
+  </si>
+  <si>
+    <t>IRR</t>
+  </si>
+  <si>
+    <t>YTM</t>
+  </si>
+  <si>
+    <t>EffAnnYield</t>
+  </si>
+  <si>
+    <t>BuyPrice</t>
+  </si>
+  <si>
+    <t>SellPrice</t>
+  </si>
+  <si>
+    <t>Dividend</t>
+  </si>
+  <si>
+    <t>Ndivs</t>
+  </si>
+  <si>
+    <t>TotRet</t>
+  </si>
+  <si>
+    <t>CapGain</t>
+  </si>
+  <si>
+    <t>DivYield</t>
+  </si>
+  <si>
+    <t>DivTot</t>
+  </si>
+  <si>
+    <t>Div1</t>
+  </si>
+  <si>
+    <t>Div2</t>
+  </si>
+  <si>
+    <t>Div3</t>
+  </si>
+  <si>
+    <t>Ret</t>
+  </si>
+  <si>
+    <t>PV1</t>
+  </si>
+  <si>
+    <t>PV2</t>
+  </si>
+  <si>
+    <t>PV3</t>
+  </si>
+  <si>
+    <t>PVTot</t>
+  </si>
+  <si>
+    <t>Shares</t>
+  </si>
+  <si>
+    <t>PVTotPerShare</t>
+  </si>
+  <si>
+    <t>StartDiv</t>
+  </si>
+  <si>
+    <t>Growth</t>
+  </si>
+  <si>
+    <t>TargRet</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>Div</t>
+  </si>
+  <si>
+    <t>DivGrowth</t>
+  </si>
+  <si>
+    <t>ImpliedGrowth</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>yrs</t>
+  </si>
+  <si>
+    <t>StartDist</t>
+  </si>
+  <si>
+    <t>LastAnnVal</t>
+  </si>
+  <si>
+    <t>NextG</t>
+  </si>
+  <si>
+    <t>NextStart</t>
+  </si>
+  <si>
+    <t>StartPerp</t>
+  </si>
+  <si>
+    <t>StartVal</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>EqPrice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,6 +297,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -133,7 +322,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -163,13 +352,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="29" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="31" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="32">
+    <cellStyle name="Comma" xfId="31" builtinId="3"/>
+    <cellStyle name="Currency" xfId="29" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -199,13 +402,160 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="30" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="47">
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -228,21 +578,21 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A49:G52" totalsRowShown="0">
-  <autoFilter ref="A49:G52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A52:G55" totalsRowShown="0">
+  <autoFilter ref="A52:G55"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Amt"/>
     <tableColumn id="2" name="APR"/>
     <tableColumn id="3" name="CompPer"/>
     <tableColumn id="4" name="Periods"/>
     <tableColumn id="5" name="RatePerPeriod">
-      <calculatedColumnFormula>$B50/$C50</calculatedColumnFormula>
+      <calculatedColumnFormula>$B53/$C53</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="TotMult">
-      <calculatedColumnFormula>POWER(1+$E50,$D50)</calculatedColumnFormula>
+      <calculatedColumnFormula>POWER(1+$E53,$D53)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="FutVal">
-      <calculatedColumnFormula>$A50*$F50</calculatedColumnFormula>
+      <calculatedColumnFormula>$A53*$F53</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -267,12 +617,193 @@
 </table>
 </file>
 
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A1:F4" totalsRowShown="0">
+  <autoFilter ref="A1:F4"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="PresVal" dataCellStyle="Currency"/>
+    <tableColumn id="2" name="FaceVal" dataCellStyle="Currency"/>
+    <tableColumn id="3" name="Nperiods" dataDxfId="45"/>
+    <tableColumn id="4" name="RetPerPeriod" dataDxfId="44" dataCellStyle="Percent">
+      <calculatedColumnFormula>POWER($B2/$A2,1/$C2)-1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="RetPeriods" dataDxfId="43"/>
+    <tableColumn id="6" name="Return" dataDxfId="42" dataCellStyle="Percent">
+      <calculatedColumnFormula>$D2*$E2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="H1:R19" totalsRowShown="0">
+  <autoFilter ref="H1:R19"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="FaceVal" dataCellStyle="Currency"/>
+    <tableColumn id="2" name="CoupVal" dataCellStyle="Currency"/>
+    <tableColumn id="3" name="CoupPerYr" dataDxfId="41"/>
+    <tableColumn id="4" name="Yrs" dataDxfId="40"/>
+    <tableColumn id="5" name="Rate" dataDxfId="39" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="PeriodRate" dataDxfId="38" dataCellStyle="Percent">
+      <calculatedColumnFormula>$L2/$J2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Nperiods" dataDxfId="37">
+      <calculatedColumnFormula>$J2*$K2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="ADF">
+      <calculatedColumnFormula>(1-1/POWER(1+$M2,$N2))/$M2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="CoupPresVal">
+      <calculatedColumnFormula>$I2*$O2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="FacePresVal">
+      <calculatedColumnFormula>$H2/POWER(1+$M2,$N2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" name="TotPresVal" dataDxfId="36" dataCellStyle="Currency">
+      <calculatedColumnFormula>$P2+$Q2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="T1:AA7" totalsRowShown="0">
+  <autoFilter ref="T1:AA7"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="TBillFaceVal" dataCellStyle="Currency"/>
+    <tableColumn id="2" name="Today" dataDxfId="35"/>
+    <tableColumn id="3" name="Maturity" dataDxfId="34"/>
+    <tableColumn id="4" name="DaysToMat">
+      <calculatedColumnFormula>$V2-$U2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Discount"/>
+    <tableColumn id="6" name="ImpliedPrice" dataDxfId="33" dataCellStyle="Currency">
+      <calculatedColumnFormula>$T2*(1-$X2*$W2/36000)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="IRR" dataDxfId="32" dataCellStyle="Percent">
+      <calculatedColumnFormula>$T2/$Y2-1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="APR" dataDxfId="31" dataCellStyle="Percent">
+      <calculatedColumnFormula>$Z2*365/$W2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="AC1:AH4" totalsRowShown="0">
+  <autoFilter ref="AC1:AH4"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="FaceVal" dataCellStyle="Currency"/>
+    <tableColumn id="2" name="PresVal" dataCellStyle="Currency"/>
+    <tableColumn id="3" name="DaysToMat"/>
+    <tableColumn id="4" name="IRR" dataDxfId="30" dataCellStyle="Percent">
+      <calculatedColumnFormula>$AC2/$AD2-1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="YTM" dataDxfId="29" dataCellStyle="Percent">
+      <calculatedColumnFormula>$AF2*360/$AE2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="EffAnnYield" dataDxfId="28" dataCellStyle="Percent">
+      <calculatedColumnFormula>POWER(1+$AG2*$AE2/365,365/$AE2)-1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table16" displayName="Table16" ref="A1:H2" totalsRowShown="0">
+  <autoFilter ref="A1:H2"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="BuyPrice" dataCellStyle="Currency"/>
+    <tableColumn id="2" name="SellPrice" dataCellStyle="Currency"/>
+    <tableColumn id="3" name="Dividend" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="Ndivs" dataDxfId="27"/>
+    <tableColumn id="5" name="DivTot" dataCellStyle="Currency">
+      <calculatedColumnFormula>$C2*$D2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="CapGain" dataDxfId="26" dataCellStyle="Percent">
+      <calculatedColumnFormula>($B2-$A2)/$A2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="DivYield" dataDxfId="25" dataCellStyle="Percent">
+      <calculatedColumnFormula>$E2/$A2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="TotRet" dataDxfId="24" dataCellStyle="Percent">
+      <calculatedColumnFormula>$F2+$G2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="J1:S2" totalsRowShown="0">
+  <autoFilter ref="J1:S2"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Div1" dataCellStyle="Currency"/>
+    <tableColumn id="2" name="Div2" dataCellStyle="Currency"/>
+    <tableColumn id="3" name="Div3" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="Ret" dataDxfId="23" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="PV1" dataDxfId="22" dataCellStyle="Currency">
+      <calculatedColumnFormula>$J2/(1+$M2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="PV2" dataDxfId="21" dataCellStyle="Currency">
+      <calculatedColumnFormula>$K2/POWER(1+$M2,2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="PV3" dataDxfId="20" dataCellStyle="Currency">
+      <calculatedColumnFormula>$L2/POWER(1+$M2,3)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="PVTotPerShare" dataDxfId="19" dataCellStyle="Currency">
+      <calculatedColumnFormula>SUM(N2:P2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="Shares" dataDxfId="18" dataCellStyle="Currency"/>
+    <tableColumn id="10" name="PVTot" dataDxfId="17" dataCellStyle="Currency">
+      <calculatedColumnFormula>$Q2*$R2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="U1:X2" totalsRowShown="0">
+  <autoFilter ref="U1:X2"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="StartDiv" dataCellStyle="Currency"/>
+    <tableColumn id="2" name="Growth" dataDxfId="16" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="TargRet" dataDxfId="15" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="PV" dataDxfId="14" dataCellStyle="Currency">
+      <calculatedColumnFormula>$U2/($W2-$V2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table19" displayName="Table19" ref="Z1:AC3" totalsRowShown="0">
+  <autoFilter ref="Z1:AC3"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="PV" dataCellStyle="Currency"/>
+    <tableColumn id="2" name="Div" dataCellStyle="Currency"/>
+    <tableColumn id="3" name="DivGrowth" dataDxfId="13" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="ImpliedGrowth" dataDxfId="12" dataCellStyle="Percent">
+      <calculatedColumnFormula>$AB2+$AA2/$Z2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="H1:L6" totalsRowShown="0">
   <autoFilter ref="H1:L6"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Loan"/>
-    <tableColumn id="2" name="Rate" dataDxfId="0">
+    <tableColumn id="2" name="Rate" dataDxfId="46">
       <calculatedColumnFormula>0.035/12</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Periods"/>
@@ -284,6 +815,99 @@
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="AE1:AO3" totalsRowShown="0">
+  <autoFilter ref="AE1:AO3"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Annuity" dataDxfId="11" dataCellStyle="Currency">
+      <calculatedColumnFormula>1.15*1.18</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="r" dataDxfId="10" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="g" dataDxfId="9" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="yrs" dataCellStyle="Comma"/>
+    <tableColumn id="5" name="ADF">
+      <calculatedColumnFormula>(POWER((1+$AG2)/(1+$AF2),$AH2)-1)/($AG2-$AF2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="StartDist" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="Discount" dataCellStyle="Comma">
+      <calculatedColumnFormula>1/POWER(1+$AF2,$AJ2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="PV" dataDxfId="8" dataCellStyle="Currency">
+      <calculatedColumnFormula>$AI2*$AE2*AK2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="LastAnnVal" dataDxfId="7" dataCellStyle="Currency">
+      <calculatedColumnFormula>$AE2*POWER(1+$AG2, $AH2-1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="NextG" dataDxfId="6" dataCellStyle="Percent"/>
+    <tableColumn id="11" name="NextStart" dataDxfId="5" dataCellStyle="Currency">
+      <calculatedColumnFormula>$AM2+$AM2*AN2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="AQ1:AW2" totalsRowShown="0">
+  <autoFilter ref="AQ1:AW2"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="StartPerp" dataCellStyle="Currency"/>
+    <tableColumn id="2" name="r" dataDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="g" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="StartVal" dataCellStyle="Currency">
+      <calculatedColumnFormula>$AQ2/($AR2-$AS2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="StartDist" dataCellStyle="Comma"/>
+    <tableColumn id="6" name="Discount" dataCellStyle="Comma">
+      <calculatedColumnFormula>1/POWER(1+$AR2,$AU2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="PV" dataDxfId="2" dataCellStyle="Currency">
+      <calculatedColumnFormula>$AT2*$AV2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table22" displayName="Table22" ref="AY1:AY5" totalsRowShown="0">
+  <autoFilter ref="AY1:AY5"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Items"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Table23" displayName="Table23" ref="BA1:BC2" totalsRowShown="0">
+  <autoFilter ref="BA1:BC2"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="EqPrice" dataCellStyle="Currency"/>
+    <tableColumn id="2" name="Div" dataCellStyle="Currency"/>
+    <tableColumn id="3" name="DivYield" dataDxfId="1" dataCellStyle="Percent">
+      <calculatedColumnFormula>$BB2/$BA2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Table24" displayName="Table24" ref="BE1:BH2" totalsRowShown="0">
+  <autoFilter ref="BE1:BH2"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="BuyPrice" dataCellStyle="Currency"/>
+    <tableColumn id="2" name="SellPrice" dataCellStyle="Currency"/>
+    <tableColumn id="3" name="Div" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="TotRet" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>($BF2-$BE2+$BG2)/$BE2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -355,8 +979,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A33:D43" totalsRowShown="0">
-  <autoFilter ref="A33:D43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A33:D46" totalsRowShown="0">
+  <autoFilter ref="A33:D46"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Perpetuity"/>
     <tableColumn id="2" name="Rate"/>
@@ -370,18 +994,18 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A45:F47" totalsRowShown="0">
-  <autoFilter ref="A45:F47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A48:F50" totalsRowShown="0">
+  <autoFilter ref="A48:F50"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Annuity"/>
     <tableColumn id="2" name="Rate"/>
     <tableColumn id="3" name="AnnGrowthRate"/>
     <tableColumn id="4" name="Periods"/>
     <tableColumn id="5" name="ADF">
-      <calculatedColumnFormula>(1-POWER((1+$C46)/(1+$B46),$D46))/($B46-$C46)</calculatedColumnFormula>
+      <calculatedColumnFormula>(1-POWER((1+$C49)/(1+$B49),$D49))/($B49-$C49)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="PresVal">
-      <calculatedColumnFormula>$A46*$E46</calculatedColumnFormula>
+      <calculatedColumnFormula>$A49*$E49</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -724,27 +1348,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA52"/>
+  <dimension ref="A1:AA55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.69921875" customWidth="1"/>
+    <col min="3" max="3" width="16.19921875" customWidth="1"/>
+    <col min="4" max="4" width="12.19921875" customWidth="1"/>
+    <col min="5" max="5" width="14.69921875" customWidth="1"/>
+    <col min="6" max="6" width="12.796875" customWidth="1"/>
+    <col min="7" max="7" width="13.796875" customWidth="1"/>
+    <col min="9" max="9" width="11.69921875" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.296875" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -806,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -817,11 +1441,11 @@
         <v>13</v>
       </c>
       <c r="D2">
-        <f>(1-1/POWER(1+$B2,$C2))/$B2</f>
+        <f t="shared" ref="D2:D9" si="0">(1-1/POWER(1+$B2,$C2))/$B2</f>
         <v>9.9856478466330501</v>
       </c>
       <c r="E2">
-        <f>$A2*$D2</f>
+        <f t="shared" ref="E2:E9" si="1">$A2*$D2</f>
         <v>9985.64784663305</v>
       </c>
       <c r="H2">
@@ -884,7 +1508,7 @@
         <v>591720.64162967331</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
@@ -895,11 +1519,11 @@
         <v>4</v>
       </c>
       <c r="D3" s="1">
-        <f>(1-1/POWER(1+$B3,$C3))/$B3</f>
+        <f t="shared" si="0"/>
         <v>3.5459505041623607</v>
       </c>
       <c r="E3" s="1">
-        <f>$A3*$D3</f>
+        <f t="shared" si="1"/>
         <v>7091.9010083247213</v>
       </c>
       <c r="F3" s="1"/>
@@ -907,7 +1531,7 @@
         <v>450000</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3" si="0">0.035/12</f>
+        <f t="shared" ref="I3" si="2">0.035/12</f>
         <v>2.9166666666666668E-3</v>
       </c>
       <c r="J3" s="1">
@@ -957,7 +1581,7 @@
         <v>4261.4113641709118</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>500</v>
       </c>
@@ -968,11 +1592,11 @@
         <v>36</v>
       </c>
       <c r="D4" s="1">
-        <f>(1-1/POWER(1+$B4,$C4))/$B4</f>
+        <f t="shared" si="0"/>
         <v>32.871016239264982</v>
       </c>
       <c r="E4" s="1">
-        <f>$A4*$D4</f>
+        <f t="shared" si="1"/>
         <v>16435.50811963249</v>
       </c>
       <c r="F4" s="1"/>
@@ -1013,7 +1637,7 @@
         <v>2743.1207247374737</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>600</v>
       </c>
@@ -1024,11 +1648,11 @@
         <v>24</v>
       </c>
       <c r="D5" s="1">
-        <f>(1-1/POWER(1+$B5,$C5))/$B5</f>
+        <f t="shared" si="0"/>
         <v>22.562866221765731</v>
       </c>
       <c r="E5" s="1">
-        <f>$A5*$D5</f>
+        <f t="shared" si="1"/>
         <v>13537.719733059439</v>
       </c>
       <c r="F5" s="1"/>
@@ -1052,7 +1676,7 @@
         <v>3064.5155066133907</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>350</v>
       </c>
@@ -1063,11 +1687,11 @@
         <v>48</v>
       </c>
       <c r="D6" s="1">
-        <f>(1-1/POWER(1+$B6,$C6))/$B6</f>
+        <f t="shared" si="0"/>
         <v>42.580317782824913</v>
       </c>
       <c r="E6" s="1">
-        <f>$A6*$D6</f>
+        <f t="shared" si="1"/>
         <v>14903.111223988719</v>
       </c>
       <c r="F6" s="1"/>
@@ -1088,7 +1712,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1000</v>
       </c>
@@ -1100,11 +1724,11 @@
         <v>40</v>
       </c>
       <c r="D7" s="1">
-        <f>(1-1/POWER(1+$B7,$C7))/$B7</f>
+        <f t="shared" si="0"/>
         <v>36.172227864082075</v>
       </c>
       <c r="E7" s="1">
-        <f>$A7*$D7</f>
+        <f t="shared" si="1"/>
         <v>36172.227864082073</v>
       </c>
       <c r="F7" s="1"/>
@@ -1114,7 +1738,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5000</v>
       </c>
@@ -1125,11 +1749,11 @@
         <v>10</v>
       </c>
       <c r="D8" s="1">
-        <f>(1-1/POWER(1+$B8,$C8))/$B8</f>
+        <f t="shared" si="0"/>
         <v>6.4176577011590128</v>
       </c>
       <c r="E8" s="1">
-        <f>$A8*$D8</f>
+        <f t="shared" si="1"/>
         <v>32088.288505795063</v>
       </c>
       <c r="F8" s="1"/>
@@ -1139,7 +1763,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>5000</v>
       </c>
@@ -1150,11 +1774,11 @@
         <v>30</v>
       </c>
       <c r="D9" s="1">
-        <f>(1-1/POWER(1+$B9,$C9))/$B9</f>
+        <f t="shared" si="0"/>
         <v>10.273654043021743</v>
       </c>
       <c r="E9" s="1">
-        <f>$A9*$D9</f>
+        <f t="shared" si="1"/>
         <v>51368.270215108714</v>
       </c>
       <c r="F9" s="1"/>
@@ -1164,7 +1788,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1172,7 +1796,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1195,7 +1819,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0.04</v>
       </c>
@@ -1203,14 +1827,14 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <f>$A13/$B13</f>
+        <f t="shared" ref="C13:C29" si="3">$A13/$B13</f>
         <v>3.3333333333333335E-3</v>
       </c>
       <c r="D13">
         <v>12</v>
       </c>
       <c r="E13">
-        <f>POWER(1+$C13,$D13)-1</f>
+        <f t="shared" ref="E13:E29" si="4">POWER(1+$C13,$D13)-1</f>
         <v>4.0741542919790819E-2</v>
       </c>
       <c r="H13">
@@ -1221,7 +1845,7 @@
         <v>6.1836546545359639E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>0.04</v>
       </c>
@@ -1229,19 +1853,19 @@
         <v>12</v>
       </c>
       <c r="C14" s="1">
-        <f>$A14/$B14</f>
+        <f t="shared" si="3"/>
         <v>3.3333333333333335E-3</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
       </c>
       <c r="E14" s="1">
-        <f>POWER(1+$C14,$D14)-1</f>
+        <f t="shared" si="4"/>
         <v>6.6777777777780045E-3</v>
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>0.04</v>
       </c>
@@ -1249,14 +1873,14 @@
         <v>12</v>
       </c>
       <c r="C15" s="1">
-        <f>$A15/$B15</f>
+        <f t="shared" si="3"/>
         <v>3.3333333333333335E-3</v>
       </c>
       <c r="D15" s="1">
         <v>3</v>
       </c>
       <c r="E15" s="1">
-        <f>POWER(1+$C15,$D15)-1</f>
+        <f t="shared" si="4"/>
         <v>1.0033370370370776E-2</v>
       </c>
       <c r="F15" s="1"/>
@@ -1270,7 +1894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>0.04</v>
       </c>
@@ -1278,14 +1902,14 @@
         <v>12</v>
       </c>
       <c r="C16" s="1">
-        <f>$A16/$B16</f>
+        <f t="shared" si="3"/>
         <v>3.3333333333333335E-3</v>
       </c>
       <c r="D16" s="1">
         <v>18</v>
       </c>
       <c r="E16" s="1">
-        <f>POWER(1+$C16,$D16)-1</f>
+        <f t="shared" si="4"/>
         <v>6.173060355153881E-2</v>
       </c>
       <c r="F16" s="1"/>
@@ -1300,7 +1924,7 @@
         <v>4.8675505653430484E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>0.06</v>
       </c>
@@ -1308,14 +1932,14 @@
         <v>2</v>
       </c>
       <c r="C17" s="1">
-        <f>$A17/$B17</f>
+        <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
       <c r="D17" s="1">
         <v>2</v>
       </c>
       <c r="E17" s="1">
-        <f>POWER(1+$C17,$D17)-1</f>
+        <f t="shared" si="4"/>
         <v>6.0899999999999954E-2</v>
       </c>
       <c r="F17" s="1"/>
@@ -1330,7 +1954,7 @@
         <v>4.0741237836483535E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>0.06</v>
       </c>
@@ -1338,19 +1962,19 @@
         <v>2</v>
       </c>
       <c r="C18" s="1">
-        <f>$A18/$B18</f>
+        <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
       <c r="D18" s="1">
         <v>0.5</v>
       </c>
       <c r="E18" s="1">
-        <f>POWER(1+$C18,$D18)-1</f>
+        <f t="shared" si="4"/>
         <v>1.4889156509221957E-2</v>
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>0.06</v>
       </c>
@@ -1358,14 +1982,14 @@
         <v>2</v>
       </c>
       <c r="C19" s="1">
-        <f>$A19/$B19</f>
+        <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
       <c r="D19" s="1">
         <v>4</v>
       </c>
       <c r="E19" s="1">
-        <f>POWER(1+$C19,$D19)-1</f>
+        <f t="shared" si="4"/>
         <v>0.12550880999999992</v>
       </c>
       <c r="F19" s="1"/>
@@ -1385,7 +2009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>0.06</v>
       </c>
@@ -1393,7 +2017,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="1">
-        <f>$A20/$B20</f>
+        <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
       <c r="D20" s="1">
@@ -1401,7 +2025,7 @@
         <v>2.5</v>
       </c>
       <c r="E20" s="1">
-        <f>POWER(1+$C20,$D20)-1</f>
+        <f t="shared" si="4"/>
         <v>7.6695906140633596E-2</v>
       </c>
       <c r="F20" s="1"/>
@@ -1423,7 +2047,7 @@
         <v>186.42959296342445</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>0.08</v>
       </c>
@@ -1431,19 +2055,19 @@
         <v>4</v>
       </c>
       <c r="C21" s="1">
-        <f>$A21/$B21</f>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
       <c r="D21" s="1">
         <v>4</v>
       </c>
       <c r="E21" s="1">
-        <f>POWER(1+$C21,$D21)-1</f>
+        <f t="shared" si="4"/>
         <v>8.2432159999999977E-2</v>
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>0.08</v>
       </c>
@@ -1451,19 +2075,19 @@
         <v>4</v>
       </c>
       <c r="C22" s="1">
-        <f>$A22/$B22</f>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
       </c>
       <c r="E22" s="1">
-        <f>POWER(1+$C22,$D22)-1</f>
+        <f t="shared" si="4"/>
         <v>4.0399999999999991E-2</v>
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>0.08</v>
       </c>
@@ -1471,19 +2095,19 @@
         <v>12</v>
       </c>
       <c r="C23" s="1">
-        <f>$A23/$B23</f>
+        <f t="shared" si="3"/>
         <v>6.6666666666666671E-3</v>
       </c>
       <c r="D23" s="1">
         <v>6</v>
       </c>
       <c r="E23" s="1">
-        <f>POWER(1+$C23,$D23)-1</f>
+        <f t="shared" si="4"/>
         <v>4.067262230132207E-2</v>
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>0.06</v>
       </c>
@@ -1491,19 +2115,19 @@
         <v>2</v>
       </c>
       <c r="C24" s="1">
-        <f>$A24/$B24</f>
+        <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
       <c r="D24" s="1">
         <v>10</v>
       </c>
       <c r="E24" s="1">
-        <f>POWER(1+$C24,$D24)-1</f>
+        <f t="shared" si="4"/>
         <v>0.34391637934412178</v>
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>0.06</v>
       </c>
@@ -1511,19 +2135,19 @@
         <v>12</v>
       </c>
       <c r="C25" s="1">
-        <f>$A25/$B25</f>
+        <f t="shared" si="3"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D25" s="1">
         <v>12</v>
       </c>
       <c r="E25" s="1">
-        <f>POWER(1+$C25,$D25)-1</f>
+        <f t="shared" si="4"/>
         <v>6.1677811864497611E-2</v>
       </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -1531,19 +2155,19 @@
         <v>4</v>
       </c>
       <c r="C26" s="1">
-        <f>$A26/$B26</f>
+        <f t="shared" si="3"/>
         <v>1.7500000000000002E-2</v>
       </c>
       <c r="D26" s="1">
         <v>4</v>
       </c>
       <c r="E26" s="1">
-        <f>POWER(1+$C26,$D26)-1</f>
+        <f t="shared" si="4"/>
         <v>7.1859031289062791E-2</v>
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>6.5000000000000002E-2</v>
       </c>
@@ -1551,19 +2175,19 @@
         <v>2</v>
       </c>
       <c r="C27" s="1">
-        <f>$A27/$B27</f>
+        <f t="shared" si="3"/>
         <v>3.2500000000000001E-2</v>
       </c>
       <c r="D27" s="1">
         <v>2</v>
       </c>
       <c r="E27" s="1">
-        <f>POWER(1+$C27,$D27)-1</f>
+        <f t="shared" si="4"/>
         <v>6.6056249999999928E-2</v>
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>0.02</v>
       </c>
@@ -1571,19 +2195,19 @@
         <v>1</v>
       </c>
       <c r="C28" s="1">
-        <f>$A28/$B28</f>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
       <c r="D28" s="1">
         <v>4</v>
       </c>
       <c r="E28" s="1">
-        <f>POWER(1+$C28,$D28)-1</f>
+        <f t="shared" si="4"/>
         <v>8.2432159999999977E-2</v>
       </c>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>0.05</v>
       </c>
@@ -1591,17 +2215,17 @@
         <v>12</v>
       </c>
       <c r="C29" s="1">
-        <f>$A29/$B29</f>
+        <f t="shared" si="3"/>
         <v>4.1666666666666666E-3</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1">
-        <f>POWER(1+$C29,$D29)-1</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1609,7 +2233,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1623,7 +2247,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1000</v>
       </c>
@@ -1634,11 +2258,11 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <f>$A34/($B34-$C34)</f>
+        <f t="shared" ref="D34:D43" si="5">$A34/($B34-$C34)</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1000</v>
       </c>
@@ -1649,11 +2273,11 @@
         <v>0.05</v>
       </c>
       <c r="D35">
-        <f>$A35/($B35-$C35)</f>
+        <f t="shared" si="5"/>
         <v>20000</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>10000</v>
       </c>
@@ -1664,11 +2288,11 @@
         <v>0</v>
       </c>
       <c r="D36" s="1">
-        <f>$A36/($B36-$C36)</f>
+        <f t="shared" si="5"/>
         <v>200000</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>1000</v>
       </c>
@@ -1679,11 +2303,11 @@
         <v>0</v>
       </c>
       <c r="D37" s="1">
-        <f>$A37/($B37-$C37)</f>
+        <f t="shared" si="5"/>
         <v>245451.5505919425</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2000</v>
       </c>
@@ -1694,11 +2318,11 @@
         <v>0.02</v>
       </c>
       <c r="D38" s="1">
-        <f>$A38/($B38-$C38)</f>
+        <f t="shared" si="5"/>
         <v>100000</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>750</v>
       </c>
@@ -1709,11 +2333,11 @@
         <v>0</v>
       </c>
       <c r="D39" s="1">
-        <f>$A39/($B39-$C39)</f>
+        <f t="shared" si="5"/>
         <v>154081.60427546428</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>500</v>
       </c>
@@ -1724,11 +2348,11 @@
         <v>1.25E-3</v>
       </c>
       <c r="D40" s="1">
-        <f>$A40/($B40-$C40)</f>
+        <f t="shared" si="5"/>
         <v>138215.06872360347</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>1000</v>
       </c>
@@ -1740,11 +2364,11 @@
         <v>0</v>
       </c>
       <c r="D41" s="1">
-        <f>$A41/($B41-$C41)</f>
+        <f t="shared" si="5"/>
         <v>240000</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>20000</v>
       </c>
@@ -1755,11 +2379,11 @@
         <v>0</v>
       </c>
       <c r="D42" s="1">
-        <f>$A42/($B42-$C42)</f>
+        <f t="shared" si="5"/>
         <v>250000</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>100</v>
       </c>
@@ -1770,172 +2394,217 @@
         <v>0.05</v>
       </c>
       <c r="D43" s="1">
-        <f>$A43/($B43-$C43)</f>
+        <f t="shared" si="5"/>
         <v>4999.9999999999991</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
-      <c r="A45" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>2</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="C44" s="1">
         <v>0</v>
       </c>
-      <c r="B45" t="s">
+      <c r="D44" s="1">
+        <f>$A44/($B44-$C44)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>3</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D45" s="1">
+        <f>$A45/($B45-$C45)</f>
+        <v>57.142857142857153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>3</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="D46" s="1">
+        <f>$A46/($B46-$C46)</f>
+        <v>70.588235294117652</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
         <v>1</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C48" t="s">
         <v>16</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D48" t="s">
         <v>2</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E48" t="s">
         <v>4</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F48" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
-      <c r="A46">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49">
         <v>90000</v>
       </c>
-      <c r="B46">
+      <c r="B49">
         <v>0.08</v>
       </c>
-      <c r="C46">
+      <c r="C49">
         <v>0.05</v>
       </c>
-      <c r="D46">
+      <c r="D49">
         <v>5</v>
       </c>
-      <c r="E46">
-        <f>(1-POWER((1+$C46)/(1+$B46),$D46))/($B46-$C46)</f>
+      <c r="E49">
+        <f>(1-POWER((1+$C49)/(1+$B49),$D49))/($B49-$C49)</f>
         <v>4.3794737959505428</v>
       </c>
-      <c r="F46">
-        <f>$A46*$E46</f>
+      <c r="F49">
+        <f>$A49*$E49</f>
         <v>394152.64163554885</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="1">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
         <v>1250</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B50" s="1">
         <v>4.8675505653430484E-3</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C50" s="1">
         <v>1.25E-3</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D50" s="1">
         <v>36</v>
       </c>
-      <c r="E47" s="1">
-        <f>(1-POWER((1+$C47)/(1+$B47),$D47))/($B47-$C47)</f>
+      <c r="E50" s="1">
+        <f>(1-POWER((1+$C50)/(1+$B50),$D50))/($B50-$C50)</f>
         <v>33.658000442053236</v>
       </c>
-      <c r="F47" s="1">
-        <f>$A47*$E47</f>
+      <c r="F50" s="1">
+        <f>$A50*$E50</f>
         <v>42072.500552566547</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
-      <c r="A49" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>17</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B52" t="s">
         <v>9</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C52" t="s">
         <v>18</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D52" t="s">
         <v>2</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E52" t="s">
         <v>19</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F52" t="s">
         <v>20</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G52" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
-      <c r="A50">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53">
         <v>1000</v>
       </c>
-      <c r="B50">
+      <c r="B53">
         <v>0.08</v>
       </c>
-      <c r="C50">
+      <c r="C53">
         <v>2</v>
       </c>
-      <c r="D50">
+      <c r="D53">
         <v>6</v>
       </c>
-      <c r="E50">
-        <f>$B50/$C50</f>
+      <c r="E53">
+        <f>$B53/$C53</f>
         <v>0.04</v>
       </c>
-      <c r="F50">
-        <f>POWER(1+$E50,$D50)</f>
+      <c r="F53">
+        <f>POWER(1+$E53,$D53)</f>
         <v>1.2653190184960004</v>
       </c>
-      <c r="G50">
-        <f>$A50*$F50</f>
+      <c r="G53">
+        <f>$A53*$F53</f>
         <v>1265.3190184960004</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="1">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
         <v>1000</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B54" s="1">
         <v>0.08</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C54" s="1">
         <v>12</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D54" s="1">
         <v>36</v>
       </c>
-      <c r="E51" s="1">
-        <f>$B51/$C51</f>
+      <c r="E54" s="1">
+        <f>$B54/$C54</f>
         <v>6.6666666666666671E-3</v>
       </c>
-      <c r="F51" s="1">
-        <f>POWER(1+$E51,$D51)</f>
+      <c r="F54" s="1">
+        <f>POWER(1+$E54,$D54)</f>
         <v>1.2702370516206511</v>
       </c>
-      <c r="G51" s="1">
-        <f>$A51*$F51</f>
+      <c r="G54" s="1">
+        <f>$A54*$F54</f>
         <v>1270.2370516206511</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="1">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
         <v>20000</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B55" s="1">
         <v>0.09</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C55" s="1">
         <v>1</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D55" s="1">
         <v>35</v>
       </c>
-      <c r="E52" s="1">
-        <f>$B52/$C52</f>
+      <c r="E55" s="1">
+        <f>$B55/$C55</f>
         <v>0.09</v>
       </c>
-      <c r="F52" s="1">
-        <f>POWER(1+$E52,$D52)</f>
+      <c r="F55" s="1">
+        <f>POWER(1+$E55,$D55)</f>
         <v>20.413967918516335</v>
       </c>
-      <c r="G52" s="1">
-        <f>$A52*$F52</f>
+      <c r="G55" s="1">
+        <f>$A55*$F55</f>
         <v>408279.35837032669</v>
       </c>
     </row>
@@ -1961,4 +2630,1658 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH19"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.09765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.69921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.19921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.3984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.19921875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.8984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.19921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.59765625" style="3" customWidth="1"/>
+    <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.8984375" customWidth="1"/>
+    <col min="23" max="23" width="12.09765625" customWidth="1"/>
+    <col min="24" max="24" width="10" customWidth="1"/>
+    <col min="25" max="25" width="15.19921875" style="3" customWidth="1"/>
+    <col min="26" max="26" width="11.796875" style="5" customWidth="1"/>
+    <col min="27" max="27" width="10" style="5" customWidth="1"/>
+    <col min="29" max="30" width="13.3984375" style="3" customWidth="1"/>
+    <col min="31" max="31" width="12.09765625" customWidth="1"/>
+    <col min="32" max="33" width="8.796875" style="5"/>
+    <col min="34" max="34" width="12.8984375" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>9492.17</v>
+      </c>
+      <c r="B2" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <f>POWER($B2/$A2,1/$C2)-1</f>
+        <v>5.3499884641762696E-2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
+        <f t="shared" ref="F2:F3" si="0">$D2*$E2</f>
+        <v>5.3499884641762696E-2</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I2" s="3">
+        <v>60</v>
+      </c>
+      <c r="J2" s="4">
+        <v>2</v>
+      </c>
+      <c r="K2" s="4">
+        <v>2</v>
+      </c>
+      <c r="L2" s="5">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="M2" s="5">
+        <f t="shared" ref="M2:M11" si="1">$L2/$J2</f>
+        <v>2.6749999999999999E-2</v>
+      </c>
+      <c r="N2" s="4">
+        <f t="shared" ref="N2:N11" si="2">$J2*$K2</f>
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ref="O2:O11" si="3">(1-1/POWER(1+$M2,$N2))/$M2</f>
+        <v>3.7461688701466742</v>
+      </c>
+      <c r="P2">
+        <f t="shared" ref="P2:P11" si="4">$I2*$O2</f>
+        <v>224.77013220880045</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2:Q11" si="5">$H2/POWER(1+$M2,$N2)</f>
+        <v>899.78998272357637</v>
+      </c>
+      <c r="R2" s="6">
+        <f t="shared" ref="R2:R11" si="6">$P2+$Q2</f>
+        <v>1124.5601149323768</v>
+      </c>
+      <c r="T2" s="3">
+        <v>100000</v>
+      </c>
+      <c r="U2" s="8">
+        <v>42528</v>
+      </c>
+      <c r="V2" s="8">
+        <v>42614</v>
+      </c>
+      <c r="W2">
+        <f t="shared" ref="W2:W7" si="7">$V2-$U2</f>
+        <v>86</v>
+      </c>
+      <c r="X2">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="Y2" s="9">
+        <f t="shared" ref="Y2:Y7" si="8">$T2*(1-$X2*$W2/36000)</f>
+        <v>99914.477777777778</v>
+      </c>
+      <c r="Z2" s="5">
+        <f t="shared" ref="Z2:Z4" si="9">$T2/$Y2-1</f>
+        <v>8.559542533208564E-4</v>
+      </c>
+      <c r="AA2" s="5">
+        <f t="shared" ref="AA2:AA4" si="10">$Z2*365/$W2</f>
+        <v>3.6328290983966578E-3</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>100000</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>98999</v>
+      </c>
+      <c r="AE2">
+        <v>54</v>
+      </c>
+      <c r="AF2" s="5">
+        <f>$AC2/$AD2-1</f>
+        <v>1.0111213244578199E-2</v>
+      </c>
+      <c r="AG2" s="5">
+        <f>$AF2*360/$AE2</f>
+        <v>6.7408088297187987E-2</v>
+      </c>
+      <c r="AH2" s="5">
+        <f>POWER(1+$AG2*$AE2/365,365/$AE2)-1</f>
+        <v>6.9374807832107255E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>455000</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="C3" s="4">
+        <v>40</v>
+      </c>
+      <c r="D3" s="5">
+        <f>POWER($B3/$A3,1/$C3)-1</f>
+        <v>1.9881502472393731E-2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5">
+        <f t="shared" si="0"/>
+        <v>3.9763004944787461E-2</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4">
+        <v>5</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M3" s="5">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="N3" s="4">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="3"/>
+        <v>3.7907867694084505</v>
+      </c>
+      <c r="P3" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="7">
+        <f t="shared" si="5"/>
+        <v>620.92132305915493</v>
+      </c>
+      <c r="R3" s="6">
+        <f t="shared" si="6"/>
+        <v>620.92132305915493</v>
+      </c>
+      <c r="T3" s="3">
+        <v>100000</v>
+      </c>
+      <c r="U3" s="8">
+        <v>42528</v>
+      </c>
+      <c r="V3" s="8">
+        <v>42614</v>
+      </c>
+      <c r="W3">
+        <f t="shared" si="7"/>
+        <v>86</v>
+      </c>
+      <c r="X3">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="Y3" s="9">
+        <f t="shared" si="8"/>
+        <v>99916.866666666669</v>
+      </c>
+      <c r="Z3" s="5">
+        <f t="shared" si="9"/>
+        <v>8.3202502346946261E-4</v>
+      </c>
+      <c r="AA3" s="5">
+        <f t="shared" si="10"/>
+        <v>3.531268994957603E-3</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>10000</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>9942.85</v>
+      </c>
+      <c r="AE3">
+        <v>81</v>
+      </c>
+      <c r="AF3" s="5">
+        <f>$AC3/$AD3-1</f>
+        <v>5.7478489567879265E-3</v>
+      </c>
+      <c r="AG3" s="5">
+        <f>$AF3*360/$AE3</f>
+        <v>2.5545995363501897E-2</v>
+      </c>
+      <c r="AH3" s="5">
+        <f>POWER(1+$AG3*$AE3/365,365/$AE3)-1</f>
+        <v>2.5801087717211013E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>744.09</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5">
+        <f>POWER($B4/$A4,1/$C4)-1</f>
+        <v>6.0901116344849404E-2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <f>$D4*$E4</f>
+        <v>6.0901116344849404E-2</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I4" s="3">
+        <v>60</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4">
+        <v>5</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M4" s="5">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="3"/>
+        <v>3.7907867694084505</v>
+      </c>
+      <c r="P4" s="7">
+        <f t="shared" si="4"/>
+        <v>227.44720616450704</v>
+      </c>
+      <c r="Q4" s="7">
+        <f t="shared" si="5"/>
+        <v>620.92132305915493</v>
+      </c>
+      <c r="R4" s="6">
+        <f t="shared" si="6"/>
+        <v>848.36852922366199</v>
+      </c>
+      <c r="T4" s="3">
+        <v>100000</v>
+      </c>
+      <c r="U4" s="8">
+        <v>42580</v>
+      </c>
+      <c r="V4" s="8">
+        <v>42824</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="7"/>
+        <v>244</v>
+      </c>
+      <c r="X4">
+        <v>0.438</v>
+      </c>
+      <c r="Y4" s="9">
+        <f t="shared" si="8"/>
+        <v>99703.133333333331</v>
+      </c>
+      <c r="Z4" s="5">
+        <f t="shared" si="9"/>
+        <v>2.9775058891496897E-3</v>
+      </c>
+      <c r="AA4" s="5">
+        <f t="shared" si="10"/>
+        <v>4.4540559407362165E-3</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>100000</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>97660</v>
+      </c>
+      <c r="AE4">
+        <v>89</v>
+      </c>
+      <c r="AF4" s="5">
+        <f>$AC4/$AD4-1</f>
+        <v>2.396067990989148E-2</v>
+      </c>
+      <c r="AG4" s="5">
+        <f>$AF4*360/$AE4</f>
+        <v>9.6919604129898126E-2</v>
+      </c>
+      <c r="AH4" s="5">
+        <f>POWER(1+$AG4*$AE4/365,365/$AE4)-1</f>
+        <v>0.10053025021471873</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="H5" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I5" s="3">
+        <v>30</v>
+      </c>
+      <c r="J5" s="4">
+        <v>2</v>
+      </c>
+      <c r="K5" s="4">
+        <v>5</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M5" s="5">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="3"/>
+        <v>7.7217349291848132</v>
+      </c>
+      <c r="P5" s="7">
+        <f t="shared" si="4"/>
+        <v>231.65204787554438</v>
+      </c>
+      <c r="Q5" s="7">
+        <f t="shared" si="5"/>
+        <v>613.91325354075934</v>
+      </c>
+      <c r="R5" s="6">
+        <f t="shared" si="6"/>
+        <v>845.56530141630378</v>
+      </c>
+      <c r="T5" s="3">
+        <v>100000</v>
+      </c>
+      <c r="U5" s="8">
+        <v>42580</v>
+      </c>
+      <c r="V5" s="8">
+        <v>42824</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="7"/>
+        <v>244</v>
+      </c>
+      <c r="X5">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="Y5" s="9">
+        <f t="shared" si="8"/>
+        <v>99709.911111111112</v>
+      </c>
+      <c r="Z5" s="5">
+        <f>$T5/$Y5-1</f>
+        <v>2.9093285276888814E-3</v>
+      </c>
+      <c r="AA5" s="5">
+        <f>$Z5*365/$W5</f>
+        <v>4.352069313960827E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="F6" s="5">
+        <f>POWER(1.06, 2)-1</f>
+        <v>0.12360000000000015</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I6" s="3">
+        <v>100</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
+        <v>4</v>
+      </c>
+      <c r="L6" s="5">
+        <v>4.4337500000000002E-2</v>
+      </c>
+      <c r="M6" s="5">
+        <f t="shared" si="1"/>
+        <v>4.4337500000000002E-2</v>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="3"/>
+        <v>3.5930935779649942</v>
+      </c>
+      <c r="P6" s="7">
+        <f t="shared" si="4"/>
+        <v>359.3093577964994</v>
+      </c>
+      <c r="Q6" s="7">
+        <f t="shared" si="5"/>
+        <v>840.69121348697706</v>
+      </c>
+      <c r="R6" s="6">
+        <f t="shared" si="6"/>
+        <v>1200.0005712834763</v>
+      </c>
+      <c r="T6" s="3">
+        <v>100000</v>
+      </c>
+      <c r="U6" s="8">
+        <v>42434</v>
+      </c>
+      <c r="V6" s="8">
+        <v>42614</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="7"/>
+        <v>180</v>
+      </c>
+      <c r="X6">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="Y6" s="9">
+        <f t="shared" si="8"/>
+        <v>99821</v>
+      </c>
+      <c r="Z6" s="5">
+        <f>$T6/$Y6-1</f>
+        <v>1.7932098456237E-3</v>
+      </c>
+      <c r="AA6" s="5">
+        <f>$Z6*365/$W6</f>
+        <v>3.6362310758480585E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="H7" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I7" s="3">
+        <v>25</v>
+      </c>
+      <c r="J7" s="4">
+        <v>4</v>
+      </c>
+      <c r="K7" s="4">
+        <v>20</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="M7" s="5">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="3"/>
+        <v>39.744513591667207</v>
+      </c>
+      <c r="P7" s="7">
+        <f t="shared" si="4"/>
+        <v>993.61283979168013</v>
+      </c>
+      <c r="Q7" s="7">
+        <f t="shared" si="5"/>
+        <v>205.10972816665586</v>
+      </c>
+      <c r="R7" s="6">
+        <f t="shared" si="6"/>
+        <v>1198.722567958336</v>
+      </c>
+      <c r="T7" s="3">
+        <v>10000</v>
+      </c>
+      <c r="U7" s="8">
+        <v>42533</v>
+      </c>
+      <c r="V7" s="8">
+        <v>42614</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="7"/>
+        <v>81</v>
+      </c>
+      <c r="X7">
+        <v>2.54</v>
+      </c>
+      <c r="Y7" s="9">
+        <f t="shared" si="8"/>
+        <v>9942.85</v>
+      </c>
+      <c r="Z7" s="5">
+        <f>$T7/$Y7-1</f>
+        <v>5.7478489567879265E-3</v>
+      </c>
+      <c r="AA7" s="5">
+        <f>$Z7*365/$W7</f>
+        <v>2.5900800854661645E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="H8" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I8" s="3">
+        <v>80</v>
+      </c>
+      <c r="J8" s="4">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4">
+        <v>20</v>
+      </c>
+      <c r="L8" s="5">
+        <v>6.2199999999999998E-2</v>
+      </c>
+      <c r="M8" s="5">
+        <f t="shared" si="1"/>
+        <v>6.2199999999999998E-2</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="3"/>
+        <v>11.26785043180219</v>
+      </c>
+      <c r="P8" s="7">
+        <f t="shared" si="4"/>
+        <v>901.42803454417515</v>
+      </c>
+      <c r="Q8" s="7">
+        <f t="shared" si="5"/>
+        <v>299.13970314190385</v>
+      </c>
+      <c r="R8" s="6">
+        <f t="shared" si="6"/>
+        <v>1200.567737686079</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="H9" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I9" s="3">
+        <v>30</v>
+      </c>
+      <c r="J9" s="4">
+        <v>2</v>
+      </c>
+      <c r="K9" s="4">
+        <v>6</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="M9" s="5">
+        <f t="shared" si="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="3"/>
+        <v>8.3838439403833256</v>
+      </c>
+      <c r="P9" s="7">
+        <f t="shared" si="4"/>
+        <v>251.51531821149976</v>
+      </c>
+      <c r="Q9" s="7">
+        <f t="shared" si="5"/>
+        <v>496.96936357700048</v>
+      </c>
+      <c r="R9" s="6">
+        <f t="shared" si="6"/>
+        <v>748.48468178850021</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="H10" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I10" s="3">
+        <v>20</v>
+      </c>
+      <c r="J10" s="4">
+        <v>2</v>
+      </c>
+      <c r="K10" s="4">
+        <v>10</v>
+      </c>
+      <c r="L10" s="5">
+        <v>5.5E-2</v>
+      </c>
+      <c r="M10" s="5">
+        <f t="shared" si="1"/>
+        <v>2.75E-2</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="3"/>
+        <v>15.227252133775616</v>
+      </c>
+      <c r="P10" s="7">
+        <f t="shared" si="4"/>
+        <v>304.54504267551232</v>
+      </c>
+      <c r="Q10" s="7">
+        <f t="shared" si="5"/>
+        <v>581.2505663211706</v>
+      </c>
+      <c r="R10" s="6">
+        <f t="shared" si="6"/>
+        <v>885.79560899668286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="H11" s="3">
+        <v>885.79560899668286</v>
+      </c>
+      <c r="I11" s="3">
+        <v>20</v>
+      </c>
+      <c r="J11" s="4">
+        <v>2</v>
+      </c>
+      <c r="K11" s="4">
+        <v>5</v>
+      </c>
+      <c r="L11" s="5">
+        <v>1.8074E-2</v>
+      </c>
+      <c r="M11" s="5">
+        <f t="shared" si="1"/>
+        <v>9.0369999999999999E-3</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="3"/>
+        <v>9.5204171880559265</v>
+      </c>
+      <c r="P11" s="7">
+        <f t="shared" si="4"/>
+        <v>190.40834376111854</v>
+      </c>
+      <c r="Q11" s="7">
+        <f t="shared" si="5"/>
+        <v>809.58528900929753</v>
+      </c>
+      <c r="R11" s="6">
+        <f t="shared" si="6"/>
+        <v>999.99363277041607</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="H12" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I12" s="3">
+        <v>50</v>
+      </c>
+      <c r="J12" s="4">
+        <v>2</v>
+      </c>
+      <c r="K12" s="4">
+        <v>5</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="M12" s="5">
+        <f t="shared" ref="M12:M19" si="11">$L12/$J12</f>
+        <v>0.02</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" ref="N12:N19" si="12">$J12*$K12</f>
+        <v>10</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ref="O12:O19" si="13">(1-1/POWER(1+$M12,$N12))/$M12</f>
+        <v>8.9825850062422337</v>
+      </c>
+      <c r="P12" s="7">
+        <f t="shared" ref="P12:P19" si="14">$I12*$O12</f>
+        <v>449.12925031211171</v>
+      </c>
+      <c r="Q12" s="7">
+        <f t="shared" ref="Q12:Q19" si="15">$H12/POWER(1+$M12,$N12)</f>
+        <v>820.34829987515525</v>
+      </c>
+      <c r="R12" s="6">
+        <f t="shared" ref="R12:R19" si="16">$P12+$Q12</f>
+        <v>1269.4775501872668</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="H13" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I13" s="3">
+        <v>90</v>
+      </c>
+      <c r="J13" s="4">
+        <v>1</v>
+      </c>
+      <c r="K13" s="4">
+        <v>10</v>
+      </c>
+      <c r="L13" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="M13" s="5">
+        <f t="shared" si="11"/>
+        <v>0.08</v>
+      </c>
+      <c r="N13" s="4">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="13"/>
+        <v>6.7100813989414476</v>
+      </c>
+      <c r="P13" s="7">
+        <f t="shared" si="14"/>
+        <v>603.90732590473033</v>
+      </c>
+      <c r="Q13" s="7">
+        <f t="shared" si="15"/>
+        <v>463.19348808468425</v>
+      </c>
+      <c r="R13" s="6">
+        <f t="shared" si="16"/>
+        <v>1067.1008139894145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="H14" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I14" s="3">
+        <v>90</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4">
+        <v>9</v>
+      </c>
+      <c r="L14" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M14" s="5">
+        <f t="shared" si="11"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="13"/>
+        <v>6.5152322487978847</v>
+      </c>
+      <c r="P14" s="7">
+        <f t="shared" si="14"/>
+        <v>586.37090239180964</v>
+      </c>
+      <c r="Q14" s="7">
+        <f t="shared" si="15"/>
+        <v>543.93374258414804</v>
+      </c>
+      <c r="R14" s="6">
+        <f t="shared" si="16"/>
+        <v>1130.3046449759577</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="H15" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>1</v>
+      </c>
+      <c r="K15" s="4">
+        <v>10</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="M15" s="5">
+        <f t="shared" si="11"/>
+        <v>0.08</v>
+      </c>
+      <c r="N15" s="4">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="13"/>
+        <v>6.7100813989414476</v>
+      </c>
+      <c r="P15" s="7">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="7">
+        <f t="shared" si="15"/>
+        <v>463.19348808468425</v>
+      </c>
+      <c r="R15" s="6">
+        <f t="shared" si="16"/>
+        <v>463.19348808468425</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="H16" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4">
+        <v>9</v>
+      </c>
+      <c r="L16" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M16" s="5">
+        <f t="shared" si="11"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N16" s="4">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="13"/>
+        <v>6.5152322487978847</v>
+      </c>
+      <c r="P16" s="7">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="7">
+        <f t="shared" si="15"/>
+        <v>543.93374258414804</v>
+      </c>
+      <c r="R16" s="6">
+        <f t="shared" si="16"/>
+        <v>543.93374258414804</v>
+      </c>
+    </row>
+    <row r="17" spans="8:18" x14ac:dyDescent="0.3">
+      <c r="H17" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I17" s="3">
+        <v>30</v>
+      </c>
+      <c r="J17" s="4">
+        <v>2</v>
+      </c>
+      <c r="K17" s="4">
+        <v>10</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="M17" s="5">
+        <f t="shared" si="11"/>
+        <v>0.04</v>
+      </c>
+      <c r="N17" s="4">
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="13"/>
+        <v>13.590326344967698</v>
+      </c>
+      <c r="P17" s="7">
+        <f t="shared" si="14"/>
+        <v>407.70979034903092</v>
+      </c>
+      <c r="Q17" s="7">
+        <f t="shared" si="15"/>
+        <v>456.38694620129206</v>
+      </c>
+      <c r="R17" s="6">
+        <f t="shared" si="16"/>
+        <v>864.09673655032293</v>
+      </c>
+    </row>
+    <row r="18" spans="8:18" x14ac:dyDescent="0.3">
+      <c r="H18" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I18" s="3">
+        <v>30</v>
+      </c>
+      <c r="J18" s="4">
+        <v>2</v>
+      </c>
+      <c r="K18" s="4">
+        <v>9</v>
+      </c>
+      <c r="L18" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M18" s="5">
+        <f t="shared" si="11"/>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="N18" s="4">
+        <f t="shared" si="12"/>
+        <v>18</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="13"/>
+        <v>13.18968172713382</v>
+      </c>
+      <c r="P18" s="7">
+        <f t="shared" si="14"/>
+        <v>395.69045181401458</v>
+      </c>
+      <c r="Q18" s="7">
+        <f t="shared" si="15"/>
+        <v>538.36113955031624</v>
+      </c>
+      <c r="R18" s="6">
+        <f t="shared" si="16"/>
+        <v>934.05159136433076</v>
+      </c>
+    </row>
+    <row r="19" spans="8:18" x14ac:dyDescent="0.3">
+      <c r="H19" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I19" s="3">
+        <v>25</v>
+      </c>
+      <c r="J19" s="4">
+        <v>4</v>
+      </c>
+      <c r="K19" s="4">
+        <v>5</v>
+      </c>
+      <c r="L19" s="5">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="M19" s="5">
+        <f t="shared" si="11"/>
+        <v>2.4750000000000001E-2</v>
+      </c>
+      <c r="N19" s="4">
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="13"/>
+        <v>15.626039927616638</v>
+      </c>
+      <c r="P19" s="7">
+        <f t="shared" si="14"/>
+        <v>390.65099819041598</v>
+      </c>
+      <c r="Q19" s="7">
+        <f t="shared" si="15"/>
+        <v>613.25551179148817</v>
+      </c>
+      <c r="R19" s="6">
+        <f t="shared" si="16"/>
+        <v>1003.9065099819042</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BH5"/>
+  <sheetViews>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AA4" sqref="AA4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.09765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.69921875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.796875" style="5"/>
+    <col min="10" max="12" width="8.796875" style="3"/>
+    <col min="13" max="13" width="8.796875" style="10"/>
+    <col min="14" max="16" width="8.796875" style="9"/>
+    <col min="17" max="17" width="10.3984375" style="9" customWidth="1"/>
+    <col min="19" max="19" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.69921875" style="3" customWidth="1"/>
+    <col min="22" max="23" width="9" style="10" customWidth="1"/>
+    <col min="24" max="24" width="8.796875" style="9"/>
+    <col min="26" max="27" width="8.796875" style="3"/>
+    <col min="28" max="28" width="11.69921875" style="10" customWidth="1"/>
+    <col min="29" max="29" width="15.296875" style="10" customWidth="1"/>
+    <col min="31" max="31" width="11.3984375" style="6" customWidth="1"/>
+    <col min="32" max="33" width="8.796875" style="10"/>
+    <col min="34" max="34" width="8.796875" style="11"/>
+    <col min="36" max="36" width="9.8984375" style="11" customWidth="1"/>
+    <col min="37" max="37" width="10" style="11" customWidth="1"/>
+    <col min="38" max="38" width="9.5" style="6" customWidth="1"/>
+    <col min="39" max="39" width="12.69921875" style="6" customWidth="1"/>
+    <col min="40" max="40" width="8.796875" style="10"/>
+    <col min="41" max="41" width="15.8984375" style="6" customWidth="1"/>
+    <col min="43" max="43" width="10.5" style="3" customWidth="1"/>
+    <col min="44" max="45" width="8.796875" style="10"/>
+    <col min="46" max="46" width="9.296875" style="3" customWidth="1"/>
+    <col min="47" max="47" width="9.8984375" style="11" customWidth="1"/>
+    <col min="48" max="48" width="10" style="11" customWidth="1"/>
+    <col min="49" max="49" width="9.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="8.796875" style="3"/>
+    <col min="55" max="55" width="9.3984375" style="10" customWidth="1"/>
+    <col min="57" max="57" width="9.796875" style="3" customWidth="1"/>
+    <col min="58" max="58" width="9.59765625" style="3" customWidth="1"/>
+    <col min="59" max="59" width="8.796875" style="3"/>
+    <col min="60" max="60" width="8.796875" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF1" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH1" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AR1" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AV1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AW1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="BB1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="BC1" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="BE1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="BF1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="BG1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="BH1" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>84.4</v>
+      </c>
+      <c r="B2" s="3">
+        <v>102.75</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <f>$C2*$D2</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F2" s="5">
+        <f>($B2-$A2)/$A2</f>
+        <v>0.21741706161137433</v>
+      </c>
+      <c r="G2" s="5">
+        <f>$E2/$A2</f>
+        <v>2.6066350710900476E-2</v>
+      </c>
+      <c r="H2" s="5">
+        <f>$F2+$G2</f>
+        <v>0.2434834123222748</v>
+      </c>
+      <c r="J2" s="3">
+        <v>20</v>
+      </c>
+      <c r="K2" s="3">
+        <v>40</v>
+      </c>
+      <c r="L2" s="3">
+        <v>35</v>
+      </c>
+      <c r="M2" s="10">
+        <v>0.09</v>
+      </c>
+      <c r="N2" s="9">
+        <f>$J2/(1+$M2)</f>
+        <v>18.348623853211009</v>
+      </c>
+      <c r="O2" s="9">
+        <f>$K2/POWER(1+$M2,2)</f>
+        <v>33.667199730662396</v>
+      </c>
+      <c r="P2" s="9">
+        <f>$L2/POWER(1+$M2,3)</f>
+        <v>27.026421802137246</v>
+      </c>
+      <c r="Q2" s="9">
+        <f>SUM(N2:P2)</f>
+        <v>79.042245386010649</v>
+      </c>
+      <c r="R2" s="9">
+        <v>5</v>
+      </c>
+      <c r="S2" s="9">
+        <f>$Q2*$R2</f>
+        <v>395.21122693005327</v>
+      </c>
+      <c r="U2" s="3">
+        <v>0.71</v>
+      </c>
+      <c r="V2" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="W2" s="10">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="X2" s="9">
+        <f>$U2/($W2-$V2)</f>
+        <v>26.296296296296298</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>80</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>5</v>
+      </c>
+      <c r="AB2" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AC2" s="10">
+        <f>$AB2+$AA2/$Z2</f>
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="AE2" s="6">
+        <f>1.15*1.18</f>
+        <v>1.3569999999999998</v>
+      </c>
+      <c r="AF2" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="AG2" s="10">
+        <v>0.18</v>
+      </c>
+      <c r="AH2" s="11">
+        <v>2</v>
+      </c>
+      <c r="AI2">
+        <f>(POWER((1+$AG2)/(1+$AF2),$AH2)-1)/($AG2-$AF2)</f>
+        <v>1.8335459183673408</v>
+      </c>
+      <c r="AJ2" s="11">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="11">
+        <f>1/POWER(1+$AF2,$AJ2)</f>
+        <v>1</v>
+      </c>
+      <c r="AL2" s="6">
+        <f>$AI2*$AE2*AK2</f>
+        <v>2.488121811224481</v>
+      </c>
+      <c r="AM2" s="6">
+        <f>$AE2*POWER(1+$AG2, $AH2-1)</f>
+        <v>1.6012599999999997</v>
+      </c>
+      <c r="AN2" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="AO2" s="6">
+        <f>$AM2+$AM2*AN2</f>
+        <v>1.8414489999999997</v>
+      </c>
+      <c r="AQ2" s="3">
+        <v>1.9519359399999996</v>
+      </c>
+      <c r="AR2" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="AS2" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="AT2" s="3">
+        <f>$AQ2/($AR2-$AS2)</f>
+        <v>32.53226566666666</v>
+      </c>
+      <c r="AU2" s="11">
+        <v>3</v>
+      </c>
+      <c r="AV2" s="11">
+        <f>1/POWER(1+$AR2,$AU2)</f>
+        <v>0.71178024781341087</v>
+      </c>
+      <c r="AW2" s="6">
+        <f>$AT2*$AV2</f>
+        <v>23.155824118151713</v>
+      </c>
+      <c r="AY2">
+        <v>2.488121811224481</v>
+      </c>
+      <c r="BA2" s="3">
+        <v>60</v>
+      </c>
+      <c r="BB2" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="BC2" s="10">
+        <f>$BB2/$BA2</f>
+        <v>2.9166666666666667E-2</v>
+      </c>
+      <c r="BE2" s="3">
+        <v>60</v>
+      </c>
+      <c r="BF2" s="3">
+        <v>69.77</v>
+      </c>
+      <c r="BG2" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="BH2" s="10">
+        <f>($BF2-$BE2+$BG2)/$BE2</f>
+        <v>0.19199999999999992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+      <c r="Z3" s="3">
+        <v>54</v>
+      </c>
+      <c r="AA3" s="3">
+        <f>3*1.04</f>
+        <v>3.12</v>
+      </c>
+      <c r="AB3" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="AC3" s="10">
+        <f>$AB3+$AA3/$Z3</f>
+        <v>9.7777777777777783E-2</v>
+      </c>
+      <c r="AE3" s="6">
+        <v>1.8414489999999997</v>
+      </c>
+      <c r="AF3" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="AG3" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="AH3" s="11">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <f>(POWER((1+$AG3)/(1+$AF3),$AH3)-1)/($AG3-$AF3)</f>
+        <v>0.89285714285713969</v>
+      </c>
+      <c r="AJ3" s="11">
+        <v>2</v>
+      </c>
+      <c r="AK3" s="11">
+        <f>1/POWER(1+$AF3,$AJ3)</f>
+        <v>0.79719387755102034</v>
+      </c>
+      <c r="AL3" s="6">
+        <f>$AI3*$AE3*AK3</f>
+        <v>1.3107070255557529</v>
+      </c>
+      <c r="AM3" s="6">
+        <f>$AE3*POWER(1+$AG3, $AH3-1)</f>
+        <v>1.8414489999999997</v>
+      </c>
+      <c r="AN3" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="AO3" s="6">
+        <f>$AM3+$AM3*AN3</f>
+        <v>1.9519359399999996</v>
+      </c>
+      <c r="AY3">
+        <v>1.3107070255557529</v>
+      </c>
+    </row>
+    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+      <c r="AY4">
+        <v>23.155824118151713</v>
+      </c>
+    </row>
+    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
+      <c r="AY5">
+        <f>SUM(AY2:AY4)</f>
+        <v>26.954652954931948</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="9">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Global markets week 3 update.
</commit_message>
<xml_diff>
--- a/ClassesTaken/Coursera/2016/InvManagementRice/01GlobalMarkets/GlobalMarkets.xlsx
+++ b/ClassesTaken/Coursera/2016/InvManagementRice/01GlobalMarkets/GlobalMarkets.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="82">
   <si>
     <t>Annuity</t>
   </si>
@@ -260,6 +260,18 @@
   </si>
   <si>
     <t>EqPrice</t>
+  </si>
+  <si>
+    <t>ContractPrice</t>
+  </si>
+  <si>
+    <t>ActualPrice</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Payoff</t>
   </si>
 </sst>
 </file>
@@ -404,7 +416,16 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="30" builtinId="5"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="50">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
@@ -578,21 +599,21 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A52:G55" totalsRowShown="0">
-  <autoFilter ref="A52:G55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A54:G57" totalsRowShown="0">
+  <autoFilter ref="A54:G57"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Amt"/>
     <tableColumn id="2" name="APR"/>
     <tableColumn id="3" name="CompPer"/>
     <tableColumn id="4" name="Periods"/>
     <tableColumn id="5" name="RatePerPeriod">
-      <calculatedColumnFormula>$B53/$C53</calculatedColumnFormula>
+      <calculatedColumnFormula>$B55/$C55</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="TotMult">
-      <calculatedColumnFormula>POWER(1+$E53,$D53)</calculatedColumnFormula>
+      <calculatedColumnFormula>POWER(1+$E55,$D55)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="FutVal">
-      <calculatedColumnFormula>$A53*$F53</calculatedColumnFormula>
+      <calculatedColumnFormula>$A55*$F55</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -623,12 +644,12 @@
   <tableColumns count="6">
     <tableColumn id="1" name="PresVal" dataCellStyle="Currency"/>
     <tableColumn id="2" name="FaceVal" dataCellStyle="Currency"/>
-    <tableColumn id="3" name="Nperiods" dataDxfId="45"/>
-    <tableColumn id="4" name="RetPerPeriod" dataDxfId="44" dataCellStyle="Percent">
+    <tableColumn id="3" name="Nperiods" dataDxfId="48"/>
+    <tableColumn id="4" name="RetPerPeriod" dataDxfId="47" dataCellStyle="Percent">
       <calculatedColumnFormula>POWER($B2/$A2,1/$C2)-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="RetPeriods" dataDxfId="43"/>
-    <tableColumn id="6" name="Return" dataDxfId="42" dataCellStyle="Percent">
+    <tableColumn id="5" name="RetPeriods" dataDxfId="46"/>
+    <tableColumn id="6" name="Return" dataDxfId="45" dataCellStyle="Percent">
       <calculatedColumnFormula>$D2*$E2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -642,13 +663,13 @@
   <tableColumns count="11">
     <tableColumn id="1" name="FaceVal" dataCellStyle="Currency"/>
     <tableColumn id="2" name="CoupVal" dataCellStyle="Currency"/>
-    <tableColumn id="3" name="CoupPerYr" dataDxfId="41"/>
-    <tableColumn id="4" name="Yrs" dataDxfId="40"/>
-    <tableColumn id="5" name="Rate" dataDxfId="39" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="PeriodRate" dataDxfId="38" dataCellStyle="Percent">
+    <tableColumn id="3" name="CoupPerYr" dataDxfId="44"/>
+    <tableColumn id="4" name="Yrs" dataDxfId="43"/>
+    <tableColumn id="5" name="Rate" dataDxfId="42" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="PeriodRate" dataDxfId="41" dataCellStyle="Percent">
       <calculatedColumnFormula>$L2/$J2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Nperiods" dataDxfId="37">
+    <tableColumn id="7" name="Nperiods" dataDxfId="40">
       <calculatedColumnFormula>$J2*$K2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="ADF">
@@ -660,7 +681,7 @@
     <tableColumn id="10" name="FacePresVal">
       <calculatedColumnFormula>$H2/POWER(1+$M2,$N2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="TotPresVal" dataDxfId="36" dataCellStyle="Currency">
+    <tableColumn id="11" name="TotPresVal" dataDxfId="39" dataCellStyle="Currency">
       <calculatedColumnFormula>$P2+$Q2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -673,19 +694,19 @@
   <autoFilter ref="T1:AA7"/>
   <tableColumns count="8">
     <tableColumn id="1" name="TBillFaceVal" dataCellStyle="Currency"/>
-    <tableColumn id="2" name="Today" dataDxfId="35"/>
-    <tableColumn id="3" name="Maturity" dataDxfId="34"/>
+    <tableColumn id="2" name="Today" dataDxfId="38"/>
+    <tableColumn id="3" name="Maturity" dataDxfId="37"/>
     <tableColumn id="4" name="DaysToMat">
       <calculatedColumnFormula>$V2-$U2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Discount"/>
-    <tableColumn id="6" name="ImpliedPrice" dataDxfId="33" dataCellStyle="Currency">
+    <tableColumn id="6" name="ImpliedPrice" dataDxfId="36" dataCellStyle="Currency">
       <calculatedColumnFormula>$T2*(1-$X2*$W2/36000)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="IRR" dataDxfId="32" dataCellStyle="Percent">
+    <tableColumn id="7" name="IRR" dataDxfId="35" dataCellStyle="Percent">
       <calculatedColumnFormula>$T2/$Y2-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="APR" dataDxfId="31" dataCellStyle="Percent">
+    <tableColumn id="8" name="APR" dataDxfId="34" dataCellStyle="Percent">
       <calculatedColumnFormula>$Z2*365/$W2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -700,13 +721,13 @@
     <tableColumn id="1" name="FaceVal" dataCellStyle="Currency"/>
     <tableColumn id="2" name="PresVal" dataCellStyle="Currency"/>
     <tableColumn id="3" name="DaysToMat"/>
-    <tableColumn id="4" name="IRR" dataDxfId="30" dataCellStyle="Percent">
+    <tableColumn id="4" name="IRR" dataDxfId="33" dataCellStyle="Percent">
       <calculatedColumnFormula>$AC2/$AD2-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="YTM" dataDxfId="29" dataCellStyle="Percent">
+    <tableColumn id="5" name="YTM" dataDxfId="32" dataCellStyle="Percent">
       <calculatedColumnFormula>$AF2*360/$AE2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="EffAnnYield" dataDxfId="28" dataCellStyle="Percent">
+    <tableColumn id="6" name="EffAnnYield" dataDxfId="31" dataCellStyle="Percent">
       <calculatedColumnFormula>POWER(1+$AG2*$AE2/365,365/$AE2)-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -721,17 +742,17 @@
     <tableColumn id="1" name="BuyPrice" dataCellStyle="Currency"/>
     <tableColumn id="2" name="SellPrice" dataCellStyle="Currency"/>
     <tableColumn id="3" name="Dividend" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="Ndivs" dataDxfId="27"/>
+    <tableColumn id="4" name="Ndivs" dataDxfId="30"/>
     <tableColumn id="5" name="DivTot" dataCellStyle="Currency">
       <calculatedColumnFormula>$C2*$D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="CapGain" dataDxfId="26" dataCellStyle="Percent">
+    <tableColumn id="6" name="CapGain" dataDxfId="29" dataCellStyle="Percent">
       <calculatedColumnFormula>($B2-$A2)/$A2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="DivYield" dataDxfId="25" dataCellStyle="Percent">
+    <tableColumn id="7" name="DivYield" dataDxfId="28" dataCellStyle="Percent">
       <calculatedColumnFormula>$E2/$A2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="TotRet" dataDxfId="24" dataCellStyle="Percent">
+    <tableColumn id="8" name="TotRet" dataDxfId="27" dataCellStyle="Percent">
       <calculatedColumnFormula>$F2+$G2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -746,21 +767,21 @@
     <tableColumn id="1" name="Div1" dataCellStyle="Currency"/>
     <tableColumn id="2" name="Div2" dataCellStyle="Currency"/>
     <tableColumn id="3" name="Div3" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="Ret" dataDxfId="23" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="PV1" dataDxfId="22" dataCellStyle="Currency">
+    <tableColumn id="4" name="Ret" dataDxfId="26" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="PV1" dataDxfId="25" dataCellStyle="Currency">
       <calculatedColumnFormula>$J2/(1+$M2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="PV2" dataDxfId="21" dataCellStyle="Currency">
+    <tableColumn id="6" name="PV2" dataDxfId="24" dataCellStyle="Currency">
       <calculatedColumnFormula>$K2/POWER(1+$M2,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="PV3" dataDxfId="20" dataCellStyle="Currency">
+    <tableColumn id="7" name="PV3" dataDxfId="23" dataCellStyle="Currency">
       <calculatedColumnFormula>$L2/POWER(1+$M2,3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="PVTotPerShare" dataDxfId="19" dataCellStyle="Currency">
+    <tableColumn id="8" name="PVTotPerShare" dataDxfId="22" dataCellStyle="Currency">
       <calculatedColumnFormula>SUM(N2:P2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Shares" dataDxfId="18" dataCellStyle="Currency"/>
-    <tableColumn id="10" name="PVTot" dataDxfId="17" dataCellStyle="Currency">
+    <tableColumn id="9" name="Shares" dataDxfId="21" dataCellStyle="Currency"/>
+    <tableColumn id="10" name="PVTot" dataDxfId="20" dataCellStyle="Currency">
       <calculatedColumnFormula>$Q2*$R2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -773,9 +794,9 @@
   <autoFilter ref="U1:X2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="StartDiv" dataCellStyle="Currency"/>
-    <tableColumn id="2" name="Growth" dataDxfId="16" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="TargRet" dataDxfId="15" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="PV" dataDxfId="14" dataCellStyle="Currency">
+    <tableColumn id="2" name="Growth" dataDxfId="19" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="TargRet" dataDxfId="18" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="PV" dataDxfId="17" dataCellStyle="Currency">
       <calculatedColumnFormula>$U2/($W2-$V2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -789,8 +810,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="PV" dataCellStyle="Currency"/>
     <tableColumn id="2" name="Div" dataCellStyle="Currency"/>
-    <tableColumn id="3" name="DivGrowth" dataDxfId="13" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="ImpliedGrowth" dataDxfId="12" dataCellStyle="Percent">
+    <tableColumn id="3" name="DivGrowth" dataDxfId="16" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="ImpliedGrowth" dataDxfId="15" dataCellStyle="Percent">
       <calculatedColumnFormula>$AB2+$AA2/$Z2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -803,7 +824,7 @@
   <autoFilter ref="H1:L6"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Loan"/>
-    <tableColumn id="2" name="Rate" dataDxfId="46">
+    <tableColumn id="2" name="Rate" dataDxfId="49">
       <calculatedColumnFormula>0.035/12</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Periods"/>
@@ -822,11 +843,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="AE1:AO3" totalsRowShown="0">
   <autoFilter ref="AE1:AO3"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Annuity" dataDxfId="11" dataCellStyle="Currency">
+    <tableColumn id="1" name="Annuity" dataDxfId="14" dataCellStyle="Currency">
       <calculatedColumnFormula>1.15*1.18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="r" dataDxfId="10" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="g" dataDxfId="9" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="r" dataDxfId="13" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="g" dataDxfId="12" dataCellStyle="Percent"/>
     <tableColumn id="4" name="yrs" dataCellStyle="Comma"/>
     <tableColumn id="5" name="ADF">
       <calculatedColumnFormula>(POWER((1+$AG2)/(1+$AF2),$AH2)-1)/($AG2-$AF2)</calculatedColumnFormula>
@@ -835,14 +856,14 @@
     <tableColumn id="7" name="Discount" dataCellStyle="Comma">
       <calculatedColumnFormula>1/POWER(1+$AF2,$AJ2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="PV" dataDxfId="8" dataCellStyle="Currency">
+    <tableColumn id="8" name="PV" dataDxfId="11" dataCellStyle="Currency">
       <calculatedColumnFormula>$AI2*$AE2*AK2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="LastAnnVal" dataDxfId="7" dataCellStyle="Currency">
+    <tableColumn id="9" name="LastAnnVal" dataDxfId="10" dataCellStyle="Currency">
       <calculatedColumnFormula>$AE2*POWER(1+$AG2, $AH2-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="NextG" dataDxfId="6" dataCellStyle="Percent"/>
-    <tableColumn id="11" name="NextStart" dataDxfId="5" dataCellStyle="Currency">
+    <tableColumn id="10" name="NextG" dataDxfId="9" dataCellStyle="Percent"/>
+    <tableColumn id="11" name="NextStart" dataDxfId="8" dataCellStyle="Currency">
       <calculatedColumnFormula>$AM2+$AM2*AN2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -855,8 +876,8 @@
   <autoFilter ref="AQ1:AW2"/>
   <tableColumns count="7">
     <tableColumn id="1" name="StartPerp" dataCellStyle="Currency"/>
-    <tableColumn id="2" name="r" dataDxfId="4" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="g" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="r" dataDxfId="7" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="g" dataDxfId="6" dataCellStyle="Percent"/>
     <tableColumn id="4" name="StartVal" dataCellStyle="Currency">
       <calculatedColumnFormula>$AQ2/($AR2-$AS2)</calculatedColumnFormula>
     </tableColumn>
@@ -864,7 +885,7 @@
     <tableColumn id="6" name="Discount" dataCellStyle="Comma">
       <calculatedColumnFormula>1/POWER(1+$AR2,$AU2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="PV" dataDxfId="2" dataCellStyle="Currency">
+    <tableColumn id="7" name="PV" dataDxfId="5" dataCellStyle="Currency">
       <calculatedColumnFormula>$AT2*$AV2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -888,7 +909,7 @@
   <tableColumns count="3">
     <tableColumn id="1" name="EqPrice" dataCellStyle="Currency"/>
     <tableColumn id="2" name="Div" dataCellStyle="Currency"/>
-    <tableColumn id="3" name="DivYield" dataDxfId="1" dataCellStyle="Percent">
+    <tableColumn id="3" name="DivYield" dataDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>$BB2/$BA2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -903,11 +924,26 @@
     <tableColumn id="1" name="BuyPrice" dataCellStyle="Currency"/>
     <tableColumn id="2" name="SellPrice" dataCellStyle="Currency"/>
     <tableColumn id="3" name="Div" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="TotRet" dataDxfId="0" dataCellStyle="Percent">
+    <tableColumn id="4" name="TotRet" dataDxfId="3" dataCellStyle="Percent">
       <calculatedColumnFormula>($BF2-$BE2+$BG2)/$BE2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Table25" displayName="Table25" ref="BJ1:BM2" totalsRowShown="0">
+  <autoFilter ref="BJ1:BM2"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="ContractPrice" dataDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="2" name="ActualPrice" dataDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="3" name="Qty" dataCellStyle="Comma"/>
+    <tableColumn id="4" name="Payoff" dataDxfId="0" dataCellStyle="Currency">
+      <calculatedColumnFormula>($BK2-$BJ2)*$BL2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -979,8 +1015,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A33:D46" totalsRowShown="0">
-  <autoFilter ref="A33:D46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A33:D48" totalsRowShown="0">
+  <autoFilter ref="A33:D48"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Perpetuity"/>
     <tableColumn id="2" name="Rate"/>
@@ -994,18 +1030,18 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A48:F50" totalsRowShown="0">
-  <autoFilter ref="A48:F50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A50:F52" totalsRowShown="0">
+  <autoFilter ref="A50:F52"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Annuity"/>
     <tableColumn id="2" name="Rate"/>
     <tableColumn id="3" name="AnnGrowthRate"/>
     <tableColumn id="4" name="Periods"/>
     <tableColumn id="5" name="ADF">
-      <calculatedColumnFormula>(1-POWER((1+$C49)/(1+$B49),$D49))/($B49-$C49)</calculatedColumnFormula>
+      <calculatedColumnFormula>(1-POWER((1+$C51)/(1+$B51),$D51))/($B51-$C51)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="PresVal">
-      <calculatedColumnFormula>$A49*$E49</calculatedColumnFormula>
+      <calculatedColumnFormula>$A51*$E51</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1348,10 +1384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA55"/>
+  <dimension ref="A1:AA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2233,7 +2269,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -2247,7 +2283,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1000</v>
       </c>
@@ -2262,7 +2298,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1000</v>
       </c>
@@ -2277,7 +2313,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>10000</v>
       </c>
@@ -2292,7 +2328,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>1000</v>
       </c>
@@ -2307,7 +2343,7 @@
         <v>245451.5505919425</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2000</v>
       </c>
@@ -2322,7 +2358,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>750</v>
       </c>
@@ -2337,7 +2373,7 @@
         <v>154081.60427546428</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>500</v>
       </c>
@@ -2352,7 +2388,7 @@
         <v>138215.06872360347</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>1000</v>
       </c>
@@ -2368,7 +2404,7 @@
         <v>240000</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>20000</v>
       </c>
@@ -2383,7 +2419,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>100</v>
       </c>
@@ -2398,7 +2434,7 @@
         <v>4999.9999999999991</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2</v>
       </c>
@@ -2413,7 +2449,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>3</v>
       </c>
@@ -2428,7 +2464,7 @@
         <v>57.142857142857153</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>3</v>
       </c>
@@ -2443,168 +2479,198 @@
         <v>70.588235294117652</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D47" s="1">
+        <f>$A47/($B47-$C47)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>2</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C48" s="1">
+        <v>7.8299999999999995E-2</v>
+      </c>
+      <c r="D48" s="1">
+        <f>$A48/($B48-$C48)</f>
+        <v>47.961630695443645</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>0</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
         <v>1</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C50" t="s">
         <v>16</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D50" t="s">
         <v>2</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E50" t="s">
         <v>4</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F50" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51">
         <v>90000</v>
       </c>
-      <c r="B49">
+      <c r="B51">
         <v>0.08</v>
       </c>
-      <c r="C49">
+      <c r="C51">
         <v>0.05</v>
       </c>
-      <c r="D49">
+      <c r="D51">
         <v>5</v>
       </c>
-      <c r="E49">
-        <f>(1-POWER((1+$C49)/(1+$B49),$D49))/($B49-$C49)</f>
+      <c r="E51">
+        <f>(1-POWER((1+$C51)/(1+$B51),$D51))/($B51-$C51)</f>
         <v>4.3794737959505428</v>
       </c>
-      <c r="F49">
-        <f>$A49*$E49</f>
+      <c r="F51">
+        <f>$A51*$E51</f>
         <v>394152.64163554885</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
         <v>1250</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B52" s="1">
         <v>4.8675505653430484E-3</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C52" s="1">
         <v>1.25E-3</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D52" s="1">
         <v>36</v>
       </c>
-      <c r="E50" s="1">
-        <f>(1-POWER((1+$C50)/(1+$B50),$D50))/($B50-$C50)</f>
+      <c r="E52" s="1">
+        <f>(1-POWER((1+$C52)/(1+$B52),$D52))/($B52-$C52)</f>
         <v>33.658000442053236</v>
       </c>
-      <c r="F50" s="1">
-        <f>$A50*$E50</f>
+      <c r="F52" s="1">
+        <f>$A52*$E52</f>
         <v>42072.500552566547</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>17</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>9</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>18</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D54" t="s">
         <v>2</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E54" t="s">
         <v>19</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F54" t="s">
         <v>20</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G54" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55">
         <v>1000</v>
       </c>
-      <c r="B53">
+      <c r="B55">
         <v>0.08</v>
       </c>
-      <c r="C53">
+      <c r="C55">
         <v>2</v>
       </c>
-      <c r="D53">
+      <c r="D55">
         <v>6</v>
       </c>
-      <c r="E53">
-        <f>$B53/$C53</f>
+      <c r="E55">
+        <f>$B55/$C55</f>
         <v>0.04</v>
       </c>
-      <c r="F53">
-        <f>POWER(1+$E53,$D53)</f>
+      <c r="F55">
+        <f>POWER(1+$E55,$D55)</f>
         <v>1.2653190184960004</v>
       </c>
-      <c r="G53">
-        <f>$A53*$F53</f>
+      <c r="G55">
+        <f>$A55*$F55</f>
         <v>1265.3190184960004</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
         <v>1000</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B56" s="1">
         <v>0.08</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C56" s="1">
         <v>12</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D56" s="1">
         <v>36</v>
       </c>
-      <c r="E54" s="1">
-        <f>$B54/$C54</f>
+      <c r="E56" s="1">
+        <f>$B56/$C56</f>
         <v>6.6666666666666671E-3</v>
       </c>
-      <c r="F54" s="1">
-        <f>POWER(1+$E54,$D54)</f>
+      <c r="F56" s="1">
+        <f>POWER(1+$E56,$D56)</f>
         <v>1.2702370516206511</v>
       </c>
-      <c r="G54" s="1">
-        <f>$A54*$F54</f>
+      <c r="G56" s="1">
+        <f>$A56*$F56</f>
         <v>1270.2370516206511</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
         <v>20000</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B57" s="1">
         <v>0.09</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C57" s="1">
         <v>1</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D57" s="1">
         <v>35</v>
       </c>
-      <c r="E55" s="1">
-        <f>$B55/$C55</f>
+      <c r="E57" s="1">
+        <f>$B57/$C57</f>
         <v>0.09</v>
       </c>
-      <c r="F55" s="1">
-        <f>POWER(1+$E55,$D55)</f>
+      <c r="F57" s="1">
+        <f>POWER(1+$E57,$D57)</f>
         <v>20.413967918516335</v>
       </c>
-      <c r="G55" s="1">
-        <f>$A55*$F55</f>
+      <c r="G57" s="1">
+        <f>$A57*$F57</f>
         <v>408279.35837032669</v>
       </c>
     </row>
@@ -3814,10 +3880,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BH5"/>
+  <dimension ref="A1:BM5"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4"/>
+    <sheetView topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3862,9 +3928,13 @@
     <col min="58" max="58" width="9.59765625" style="3" customWidth="1"/>
     <col min="59" max="59" width="8.796875" style="3"/>
     <col min="60" max="60" width="8.796875" style="10"/>
+    <col min="62" max="62" width="13.8984375" style="6" customWidth="1"/>
+    <col min="63" max="63" width="12" style="6" customWidth="1"/>
+    <col min="64" max="64" width="9.09765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="10.59765625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>42</v>
       </c>
@@ -4021,8 +4091,20 @@
       <c r="BH1" s="10" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
+      <c r="BJ1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="BK1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="BL1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="BM1" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>84.4</v>
       </c>
@@ -4201,8 +4283,21 @@
         <f>($BF2-$BE2+$BG2)/$BE2</f>
         <v>0.19199999999999992</v>
       </c>
-    </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+      <c r="BJ2" s="6">
+        <v>3.9020000000000001</v>
+      </c>
+      <c r="BK2" s="6">
+        <v>4.0994999999999999</v>
+      </c>
+      <c r="BL2" s="11">
+        <v>5000</v>
+      </c>
+      <c r="BM2" s="6">
+        <f>($BK2-$BJ2)*$BL2</f>
+        <v>987.49999999999898</v>
+      </c>
+    </row>
+    <row r="3" spans="1:65" x14ac:dyDescent="0.3">
       <c r="Z3" s="3">
         <v>54</v>
       </c>
@@ -4259,12 +4354,12 @@
         <v>1.3107070255557529</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.3">
       <c r="AY4">
         <v>23.155824118151713</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
       <c r="AY5">
         <f>SUM(AY2:AY4)</f>
         <v>26.954652954931948</v>
@@ -4272,7 +4367,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="9">
+  <tableParts count="10">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -4282,6 +4377,7 @@
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>